<commit_message>
New models, modified EXP2 sim and fit to sim script
</commit_message>
<xml_diff>
--- a/comparative_models/results/variable_feedback/model_comparison/model_and_param_recovery/model_fits_EXP2_sim_test.xlsx
+++ b/comparative_models/results/variable_feedback/model_comparison/model_and_param_recovery/model_fits_EXP2_sim_test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BX9"/>
+  <dimension ref="A1:CU12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -731,82 +731,197 @@
       </c>
       <c r="BI1" s="1" t="inlineStr">
         <is>
-          <t>w_rw_rwp</t>
+          <t>wp_rwp</t>
         </is>
       </c>
       <c r="BJ1" s="1" t="inlineStr">
         <is>
-          <t>w_performance_rwp</t>
+          <t>nll_rwp</t>
         </is>
       </c>
       <c r="BK1" s="1" t="inlineStr">
         <is>
-          <t>intercept_rwp</t>
+          <t>aic_rwp</t>
         </is>
       </c>
       <c r="BL1" s="1" t="inlineStr">
         <is>
-          <t>nll_rwp</t>
+          <t>bic_rwp</t>
         </is>
       </c>
       <c r="BM1" s="1" t="inlineStr">
         <is>
-          <t>aic_rwp</t>
+          <t>pseudo_r2_rwp</t>
         </is>
       </c>
       <c r="BN1" s="1" t="inlineStr">
         <is>
-          <t>bic_rwp</t>
+          <t>alpha_rwfp</t>
         </is>
       </c>
       <c r="BO1" s="1" t="inlineStr">
         <is>
-          <t>pseudo_r2_rwp</t>
+          <t>sigma_rwfp</t>
         </is>
       </c>
       <c r="BP1" s="1" t="inlineStr">
         <is>
-          <t>alpha_rwpd</t>
+          <t>bias_rwfp</t>
         </is>
       </c>
       <c r="BQ1" s="1" t="inlineStr">
         <is>
-          <t>sigma_rwpd</t>
+          <t>wf_rwfp</t>
         </is>
       </c>
       <c r="BR1" s="1" t="inlineStr">
         <is>
-          <t>bias_rwpd</t>
+          <t>wp_rwfp</t>
         </is>
       </c>
       <c r="BS1" s="1" t="inlineStr">
         <is>
-          <t>w_rw_rwpd</t>
+          <t>nll_rwfp</t>
         </is>
       </c>
       <c r="BT1" s="1" t="inlineStr">
         <is>
-          <t>w_pd_rwpd</t>
+          <t>aic_rwfp</t>
         </is>
       </c>
       <c r="BU1" s="1" t="inlineStr">
         <is>
-          <t>nll_rwpd</t>
+          <t>bic_rwfp</t>
         </is>
       </c>
       <c r="BV1" s="1" t="inlineStr">
         <is>
-          <t>aic_rwpd</t>
+          <t>pseudo_r2_rwfp</t>
         </is>
       </c>
       <c r="BW1" s="1" t="inlineStr">
         <is>
-          <t>bic_rwpd</t>
+          <t>sigma_lmf</t>
         </is>
       </c>
       <c r="BX1" s="1" t="inlineStr">
         <is>
-          <t>pseudo_r2_rwpd</t>
+          <t>bias_lmf</t>
+        </is>
+      </c>
+      <c r="BY1" s="1" t="inlineStr">
+        <is>
+          <t>intercept_lmf</t>
+        </is>
+      </c>
+      <c r="BZ1" s="1" t="inlineStr">
+        <is>
+          <t>wf_lmf</t>
+        </is>
+      </c>
+      <c r="CA1" s="1" t="inlineStr">
+        <is>
+          <t>nll_lmf</t>
+        </is>
+      </c>
+      <c r="CB1" s="1" t="inlineStr">
+        <is>
+          <t>aic_lmf</t>
+        </is>
+      </c>
+      <c r="CC1" s="1" t="inlineStr">
+        <is>
+          <t>bic_lmf</t>
+        </is>
+      </c>
+      <c r="CD1" s="1" t="inlineStr">
+        <is>
+          <t>pseudo_r2_lmf</t>
+        </is>
+      </c>
+      <c r="CE1" s="1" t="inlineStr">
+        <is>
+          <t>sigma_lmp</t>
+        </is>
+      </c>
+      <c r="CF1" s="1" t="inlineStr">
+        <is>
+          <t>bias_lmp</t>
+        </is>
+      </c>
+      <c r="CG1" s="1" t="inlineStr">
+        <is>
+          <t>intercept_lmp</t>
+        </is>
+      </c>
+      <c r="CH1" s="1" t="inlineStr">
+        <is>
+          <t>wp_lmp</t>
+        </is>
+      </c>
+      <c r="CI1" s="1" t="inlineStr">
+        <is>
+          <t>nll_lmp</t>
+        </is>
+      </c>
+      <c r="CJ1" s="1" t="inlineStr">
+        <is>
+          <t>aic_lmp</t>
+        </is>
+      </c>
+      <c r="CK1" s="1" t="inlineStr">
+        <is>
+          <t>bic_lmp</t>
+        </is>
+      </c>
+      <c r="CL1" s="1" t="inlineStr">
+        <is>
+          <t>pseudo_r2_lmp</t>
+        </is>
+      </c>
+      <c r="CM1" s="1" t="inlineStr">
+        <is>
+          <t>sigma_lmfp</t>
+        </is>
+      </c>
+      <c r="CN1" s="1" t="inlineStr">
+        <is>
+          <t>bias_lmfp</t>
+        </is>
+      </c>
+      <c r="CO1" s="1" t="inlineStr">
+        <is>
+          <t>intercept_lmfp</t>
+        </is>
+      </c>
+      <c r="CP1" s="1" t="inlineStr">
+        <is>
+          <t>wf_lmfp</t>
+        </is>
+      </c>
+      <c r="CQ1" s="1" t="inlineStr">
+        <is>
+          <t>wp_lmfp</t>
+        </is>
+      </c>
+      <c r="CR1" s="1" t="inlineStr">
+        <is>
+          <t>nll_lmfp</t>
+        </is>
+      </c>
+      <c r="CS1" s="1" t="inlineStr">
+        <is>
+          <t>aic_lmfp</t>
+        </is>
+      </c>
+      <c r="CT1" s="1" t="inlineStr">
+        <is>
+          <t>bic_lmfp</t>
+        </is>
+      </c>
+      <c r="CU1" s="1" t="inlineStr">
+        <is>
+          <t>pseudo_r2_lmfp</t>
         </is>
       </c>
     </row>
@@ -845,205 +960,274 @@
         <v>10.83967894611662</v>
       </c>
       <c r="J2" t="n">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>34.27777764724485</v>
+        <v>21.99641937238431</v>
       </c>
       <c r="L2" t="n">
-        <v>1</v>
+        <v>4.331527135570259</v>
       </c>
       <c r="M2" t="n">
-        <v>2.312456854682838</v>
+        <v>10.4629498422478</v>
       </c>
       <c r="N2" t="n">
-        <v>8.624913709365677</v>
+        <v>24.92589968449561</v>
       </c>
       <c r="O2" t="n">
-        <v>7.843789534233878</v>
+        <v>24.14477550936381</v>
       </c>
       <c r="P2" t="n">
-        <v>0.9119276951306073</v>
+        <v>-1.267102192470803</v>
       </c>
       <c r="Q2" t="n">
-        <v>3.364671500833061</v>
+        <v>4.662704915061436</v>
       </c>
       <c r="R2" t="n">
-        <v>51.6050632555698</v>
+        <v>49.56240827595483</v>
       </c>
       <c r="S2" t="n">
-        <v>2.220669445989339</v>
+        <v>4.158813488944029</v>
       </c>
       <c r="T2" t="n">
-        <v>8.441338891978678</v>
+        <v>12.31762697788806</v>
       </c>
       <c r="U2" t="n">
-        <v>7.660214716846878</v>
+        <v>11.53650280275626</v>
       </c>
       <c r="V2" t="n">
-        <v>0.6119120454796111</v>
+        <v>0.09887218031080625</v>
       </c>
       <c r="W2" t="n">
-        <v>0.01866813581045064</v>
+        <v>0.1279150864633629</v>
       </c>
       <c r="X2" t="n">
-        <v>1.293716598131354</v>
+        <v>7.74320797372567</v>
       </c>
       <c r="Y2" t="n">
-        <v>33.0727350517534</v>
+        <v>13.58377963307905</v>
       </c>
       <c r="Z2" t="n">
-        <v>1.189089733418746</v>
+        <v>7.129367209022742</v>
       </c>
       <c r="AA2" t="n">
-        <v>8.378179466837492</v>
+        <v>20.25873441804548</v>
       </c>
       <c r="AB2" t="n">
-        <v>7.20649320413979</v>
+        <v>19.08704815534778</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.8783192186808856</v>
+        <v>-0.5447846232848357</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.1036114069616119</v>
+        <v>0.4124774666169024</v>
       </c>
       <c r="AE2" t="n">
-        <v>0.01588201163141132</v>
+        <v>0.001273146698544244</v>
       </c>
       <c r="AF2" t="n">
-        <v>0.2826591551204099</v>
+        <v>0.2468015236161851</v>
       </c>
       <c r="AG2" t="n">
-        <v>1.080689431597324</v>
+        <v>6.361471997719504</v>
       </c>
       <c r="AH2" t="n">
-        <v>29.06579240205126</v>
+        <v>41.1777570763936</v>
       </c>
       <c r="AI2" t="n">
-        <v>1.503899116383982</v>
+        <v>8.003905602940138</v>
       </c>
       <c r="AJ2" t="n">
-        <v>13.00779823276796</v>
+        <v>26.00781120588028</v>
       </c>
       <c r="AK2" t="n">
-        <v>11.05498779493846</v>
+        <v>24.05500076805078</v>
       </c>
       <c r="AL2" t="n">
-        <v>0.8856135054564556</v>
+        <v>-0.7342787850788944</v>
       </c>
       <c r="AM2" t="n">
-        <v>0.722761045675408</v>
+        <v>0.7372622976828668</v>
       </c>
       <c r="AN2" t="n">
-        <v>9.429069803871833</v>
+        <v>9.561393641291646</v>
       </c>
       <c r="AO2" t="n">
-        <v>80.02602290051598</v>
+        <v>52.47712242079964</v>
       </c>
       <c r="AP2" t="n">
-        <v>185.4702291617672</v>
+        <v>166.5892618993543</v>
       </c>
       <c r="AQ2" t="n">
-        <v>2.408658254286379</v>
+        <v>5.109796452979965</v>
       </c>
       <c r="AR2" t="n">
-        <v>12.81731650857276</v>
+        <v>18.21959290595993</v>
       </c>
       <c r="AS2" t="n">
-        <v>11.25506815830916</v>
+        <v>16.65734455569633</v>
       </c>
       <c r="AT2" t="n">
-        <v>0.7563310042634056</v>
+        <v>-0.1071859194865137</v>
       </c>
       <c r="AU2" t="n">
-        <v>0.3452100677730697</v>
+        <v>0.1716526336529191</v>
       </c>
       <c r="AV2" t="n">
-        <v>0</v>
+        <v>0.6488549011926432</v>
       </c>
       <c r="AW2" t="n">
-        <v>10.96410450768179</v>
+        <v>9.972125449254937</v>
       </c>
       <c r="AX2" t="n">
-        <v>15</v>
+        <v>4.467907279785373</v>
       </c>
       <c r="AY2" t="n">
-        <v>52.52630718330113</v>
+        <v>38.96113081870985</v>
       </c>
       <c r="AZ2" t="n">
-        <v>101.3169125778275</v>
+        <v>85.65375855759042</v>
       </c>
       <c r="BA2" t="n">
-        <v>51.01881290730442</v>
+        <v>175.5878994799405</v>
       </c>
       <c r="BB2" t="n">
-        <v>5.322980482879665</v>
+        <v>4.737052924372078</v>
       </c>
       <c r="BC2" t="n">
-        <v>24.64596096575933</v>
+        <v>23.47410584874416</v>
       </c>
       <c r="BD2" t="n">
-        <v>21.91202635279803</v>
+        <v>20.74017123578286</v>
       </c>
       <c r="BE2" t="n">
-        <v>0.7009653054659868</v>
+        <v>-0.02642020009788885</v>
       </c>
       <c r="BF2" t="n">
-        <v>0.2492172299293875</v>
+        <v>0.1977902510450578</v>
       </c>
       <c r="BG2" t="n">
-        <v>5.811357001086865</v>
+        <v>3.550531362686103</v>
       </c>
       <c r="BH2" t="n">
-        <v>14.13529473658903</v>
+        <v>50.59787966825763</v>
       </c>
       <c r="BI2" t="n">
-        <v>0.2682615784957137</v>
+        <v>0.5286892362084918</v>
       </c>
       <c r="BJ2" t="n">
-        <v>0.38888644167274</v>
+        <v>3.234310225419132</v>
       </c>
       <c r="BK2" t="n">
-        <v>0.38888644167274</v>
+        <v>14.46862045083826</v>
       </c>
       <c r="BL2" t="n">
-        <v>18.44571606857103</v>
+        <v>12.90637210057466</v>
       </c>
       <c r="BM2" t="n">
-        <v>4.550470432477503</v>
+        <v>0.2991926833510298</v>
       </c>
       <c r="BN2" t="n">
-        <v>21.10094086495501</v>
+        <v>0.6632940991297448</v>
       </c>
       <c r="BO2" t="n">
-        <v>18.75756833955961</v>
+        <v>2.500407984355661</v>
       </c>
       <c r="BP2" t="n">
-        <v>0.8316539804305402</v>
+        <v>38.62709620752303</v>
       </c>
       <c r="BQ2" t="n">
-        <v>10.98519718779018</v>
+        <v>1.594991214172605</v>
       </c>
       <c r="BR2" t="n">
-        <v>60.18117356445904</v>
+        <v>1.230659612525875</v>
       </c>
       <c r="BS2" t="n">
-        <v>0.4464735824004478</v>
+        <v>1.620975006954179</v>
       </c>
       <c r="BT2" t="n">
-        <v>3.558441105634475</v>
+        <v>13.24195001390836</v>
       </c>
       <c r="BU2" t="n">
-        <v>4.264199742359919</v>
+        <v>11.28913957607886</v>
       </c>
       <c r="BV2" t="n">
-        <v>18.52839948471984</v>
+        <v>0.6487686505609115</v>
       </c>
       <c r="BW2" t="n">
-        <v>16.57558904689034</v>
+        <v>5.845881228720065</v>
       </c>
       <c r="BX2" t="n">
-        <v>0.02793050086388523</v>
+        <v>52.2612009632632</v>
+      </c>
+      <c r="BY2" t="n">
+        <v>18.70480928205481</v>
+      </c>
+      <c r="BZ2" t="n">
+        <v>0.04877145883491937</v>
+      </c>
+      <c r="CA2" t="n">
+        <v>4.644606898777519</v>
+      </c>
+      <c r="CB2" t="n">
+        <v>17.28921379755504</v>
+      </c>
+      <c r="CC2" t="n">
+        <v>15.72696544729144</v>
+      </c>
+      <c r="CD2" t="n">
+        <v>-0.006389081678075208</v>
+      </c>
+      <c r="CE2" t="n">
+        <v>4.027774795946098</v>
+      </c>
+      <c r="CF2" t="n">
+        <v>67.29433446419984</v>
+      </c>
+      <c r="CG2" t="n">
+        <v>51.99011291914755</v>
+      </c>
+      <c r="CH2" t="n">
+        <v>0.751721875992882</v>
+      </c>
+      <c r="CI2" t="n">
+        <v>3.168762512278791</v>
+      </c>
+      <c r="CJ2" t="n">
+        <v>14.33752502455758</v>
+      </c>
+      <c r="CK2" t="n">
+        <v>12.77527667429398</v>
+      </c>
+      <c r="CL2" t="n">
+        <v>0.3133955005691605</v>
+      </c>
+      <c r="CM2" t="n">
+        <v>7.031959493382327</v>
+      </c>
+      <c r="CN2" t="n">
+        <v>71.03181080540476</v>
+      </c>
+      <c r="CO2" t="n">
+        <v>13.6002261299517</v>
+      </c>
+      <c r="CP2" t="n">
+        <v>0.5719423884114945</v>
+      </c>
+      <c r="CQ2" t="n">
+        <v>0.2810814943471017</v>
+      </c>
+      <c r="CR2" t="n">
+        <v>3.558627399061459</v>
+      </c>
+      <c r="CS2" t="n">
+        <v>17.11725479812292</v>
+      </c>
+      <c r="CT2" t="n">
+        <v>15.16444436029342</v>
+      </c>
+      <c r="CU2" t="n">
+        <v>0.2289199412939492</v>
       </c>
     </row>
     <row r="3">
@@ -1081,205 +1265,274 @@
         <v>10.83967894611662</v>
       </c>
       <c r="J3" t="n">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>53.10337366079324</v>
+        <v>72.7834252959354</v>
       </c>
       <c r="L3" t="n">
-        <v>6.282435110101455</v>
+        <v>1.16621749142142</v>
       </c>
       <c r="M3" t="n">
-        <v>10.029642174755</v>
+        <v>2.022424167518886</v>
       </c>
       <c r="N3" t="n">
-        <v>24.05928434951</v>
+        <v>8.044848335037772</v>
       </c>
       <c r="O3" t="n">
-        <v>23.27816017437821</v>
+        <v>7.263724159905974</v>
       </c>
       <c r="P3" t="n">
-        <v>0.4287185950154089</v>
+        <v>0.5617830216700169</v>
       </c>
       <c r="Q3" t="n">
-        <v>5.348940447089327</v>
+        <v>1.096998206788212</v>
       </c>
       <c r="R3" t="n">
-        <v>32.43049685856391</v>
+        <v>61.97491619522549</v>
       </c>
       <c r="S3" t="n">
-        <v>3.360916126207407</v>
+        <v>2.070742744300211</v>
       </c>
       <c r="T3" t="n">
-        <v>10.72183225241481</v>
+        <v>8.141485488600422</v>
       </c>
       <c r="U3" t="n">
-        <v>9.940708077283013</v>
+        <v>7.360361313468623</v>
       </c>
       <c r="V3" t="n">
-        <v>0.7024821144648916</v>
+        <v>0.5513133976146964</v>
       </c>
       <c r="W3" t="n">
-        <v>0.1304947537014638</v>
+        <v>0.2228173534027206</v>
       </c>
       <c r="X3" t="n">
-        <v>5.883356085632621</v>
+        <v>1.41185722712988</v>
       </c>
       <c r="Y3" t="n">
-        <v>49.37568513649189</v>
+        <v>62.31216852678415</v>
       </c>
       <c r="Z3" t="n">
-        <v>3.500059334597694</v>
+        <v>1.278289474494573</v>
       </c>
       <c r="AA3" t="n">
-        <v>13.00011866919539</v>
+        <v>8.556578948989147</v>
       </c>
       <c r="AB3" t="n">
-        <v>11.82843240649769</v>
+        <v>7.384892686291447</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.4287185950520477</v>
+        <v>0.723021431438268</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.4520087953727492</v>
+        <v>0.8514208011641945</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.199682070740747</v>
+        <v>0.2869411761883172</v>
       </c>
       <c r="AF3" t="n">
-        <v>0.4773722766594529</v>
+        <v>0.2308828920074515</v>
       </c>
       <c r="AG3" t="n">
-        <v>4.612404899283816</v>
+        <v>1.31283257770275</v>
       </c>
       <c r="AH3" t="n">
-        <v>30.02018305837077</v>
+        <v>50.20232891922621</v>
       </c>
       <c r="AI3" t="n">
-        <v>2.538455096026514</v>
+        <v>1.645098227479356</v>
       </c>
       <c r="AJ3" t="n">
-        <v>15.07691019205303</v>
+        <v>13.29019645495871</v>
       </c>
       <c r="AK3" t="n">
-        <v>13.12409975422353</v>
+        <v>11.33738601712921</v>
       </c>
       <c r="AL3" t="n">
-        <v>0.4384927279549823</v>
+        <v>0.6435416536846331</v>
       </c>
       <c r="AM3" t="n">
-        <v>0.8969932137138695</v>
+        <v>0.6278463831053923</v>
       </c>
       <c r="AN3" t="n">
-        <v>13.33257542382003</v>
+        <v>4.196463895606116</v>
       </c>
       <c r="AO3" t="n">
-        <v>39.85909108673206</v>
+        <v>70.37351892038929</v>
       </c>
       <c r="AP3" t="n">
-        <v>198.1772887345712</v>
+        <v>195.1377126227395</v>
       </c>
       <c r="AQ3" t="n">
-        <v>4.259558635451017</v>
+        <v>2.150261617016683</v>
       </c>
       <c r="AR3" t="n">
-        <v>16.51911727090203</v>
+        <v>12.30052323403337</v>
       </c>
       <c r="AS3" t="n">
-        <v>14.95686892063844</v>
+        <v>10.73827488376977</v>
       </c>
       <c r="AT3" t="n">
-        <v>0.6949781345067737</v>
+        <v>0.5340833225979561</v>
       </c>
       <c r="AU3" t="n">
-        <v>0.8306031261968134</v>
+        <v>0.7656838901781917</v>
       </c>
       <c r="AV3" t="n">
-        <v>0.0965221171613156</v>
+        <v>0.5854818325165435</v>
       </c>
       <c r="AW3" t="n">
-        <v>10.50284380488672</v>
+        <v>4.989361289297934</v>
       </c>
       <c r="AX3" t="n">
-        <v>12.50637411811877</v>
+        <v>4.693334837606478</v>
       </c>
       <c r="AY3" t="n">
-        <v>35.92927928139004</v>
+        <v>38.07071204383998</v>
       </c>
       <c r="AZ3" t="n">
-        <v>99.70509751605016</v>
+        <v>116.4750539709461</v>
       </c>
       <c r="BA3" t="n">
-        <v>49.48133510295302</v>
+        <v>154.0813669698048</v>
       </c>
       <c r="BB3" t="n">
-        <v>5.346537110274039</v>
+        <v>2.659030994138061</v>
       </c>
       <c r="BC3" t="n">
-        <v>24.69307422054808</v>
+        <v>19.31806198827612</v>
       </c>
       <c r="BD3" t="n">
-        <v>21.95913960758678</v>
+        <v>16.58412737531483</v>
       </c>
       <c r="BE3" t="n">
-        <v>0.6524846633145386</v>
+        <v>0.4238436494919554</v>
       </c>
       <c r="BF3" t="n">
-        <v>0.6506029595590762</v>
+        <v>0.002417720100263808</v>
       </c>
       <c r="BG3" t="n">
-        <v>1.34455377306061</v>
+        <v>1.295221665519072</v>
       </c>
       <c r="BH3" t="n">
-        <v>87.92280285973391</v>
+        <v>73.31395951204162</v>
       </c>
       <c r="BI3" t="n">
-        <v>0.2102903600134141</v>
+        <v>0.6031805877233919</v>
       </c>
       <c r="BJ3" t="n">
-        <v>0.4284187469234602</v>
+        <v>1.992372603495895</v>
       </c>
       <c r="BK3" t="n">
-        <v>0.4284187469234602</v>
+        <v>11.98474520699179</v>
       </c>
       <c r="BL3" t="n">
-        <v>20.83712623051801</v>
+        <v>10.42249685672819</v>
       </c>
       <c r="BM3" t="n">
-        <v>1.843799373827177</v>
+        <v>0.5682945664743898</v>
       </c>
       <c r="BN3" t="n">
-        <v>15.68759874765435</v>
+        <v>0.02032840817472783</v>
       </c>
       <c r="BO3" t="n">
-        <v>13.34422622225895</v>
+        <v>1</v>
       </c>
       <c r="BP3" t="n">
-        <v>0.6765312367886871</v>
+        <v>71.25972421524786</v>
       </c>
       <c r="BQ3" t="n">
-        <v>10.78791595256511</v>
+        <v>0.5470913078124195</v>
       </c>
       <c r="BR3" t="n">
-        <v>30.78017729886047</v>
+        <v>1.705536883434502</v>
       </c>
       <c r="BS3" t="n">
-        <v>0.8037570707241297</v>
+        <v>1.498249340104278</v>
       </c>
       <c r="BT3" t="n">
-        <v>3.320783272473556</v>
+        <v>12.99649868020856</v>
       </c>
       <c r="BU3" t="n">
-        <v>7.20046326406536</v>
+        <v>11.04368824237906</v>
       </c>
       <c r="BV3" t="n">
-        <v>24.40092652813072</v>
+        <v>0.6753607333466279</v>
       </c>
       <c r="BW3" t="n">
-        <v>22.44811609030122</v>
+        <v>1.220123305679244</v>
       </c>
       <c r="BX3" t="n">
-        <v>-0.02398022114251463</v>
+        <v>18.72594540794611</v>
+      </c>
+      <c r="BY3" t="n">
+        <v>69.97207270817798</v>
+      </c>
+      <c r="BZ3" t="n">
+        <v>0.04156874371291587</v>
+      </c>
+      <c r="CA3" t="n">
+        <v>1.412986272879738</v>
+      </c>
+      <c r="CB3" t="n">
+        <v>10.82597254575948</v>
+      </c>
+      <c r="CC3" t="n">
+        <v>9.263724195495879</v>
+      </c>
+      <c r="CD3" t="n">
+        <v>0.6938354550604817</v>
+      </c>
+      <c r="CE3" t="n">
+        <v>1.000000019738538</v>
+      </c>
+      <c r="CF3" t="n">
+        <v>13.90464725001954</v>
+      </c>
+      <c r="CG3" t="n">
+        <v>72.77777763930125</v>
+      </c>
+      <c r="CH3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CI3" t="n">
+        <v>2.048567929912355</v>
+      </c>
+      <c r="CJ3" t="n">
+        <v>12.09713585982471</v>
+      </c>
+      <c r="CK3" t="n">
+        <v>10.53488750956111</v>
+      </c>
+      <c r="CL3" t="n">
+        <v>0.5561182156702461</v>
+      </c>
+      <c r="CM3" t="n">
+        <v>4</v>
+      </c>
+      <c r="CN3" t="n">
+        <v>46.07199936119087</v>
+      </c>
+      <c r="CO3" t="n">
+        <v>58.28360451543701</v>
+      </c>
+      <c r="CP3" t="n">
+        <v>0.377568668169908</v>
+      </c>
+      <c r="CQ3" t="n">
+        <v>0.4906156172177867</v>
+      </c>
+      <c r="CR3" t="n">
+        <v>2.374026984242862</v>
+      </c>
+      <c r="CS3" t="n">
+        <v>14.74805396848573</v>
+      </c>
+      <c r="CT3" t="n">
+        <v>12.79524353065623</v>
+      </c>
+      <c r="CU3" t="n">
+        <v>0.4855980519729257</v>
       </c>
     </row>
     <row r="4">
@@ -1317,205 +1570,274 @@
         <v>10.83967894611662</v>
       </c>
       <c r="J4" t="n">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>54.86072103140675</v>
+        <v>80.36824035661685</v>
       </c>
       <c r="L4" t="n">
-        <v>2.639884378285466</v>
+        <v>7.047026392936495</v>
       </c>
       <c r="M4" t="n">
-        <v>6.072273608403425</v>
+        <v>9.084318228600653</v>
       </c>
       <c r="N4" t="n">
-        <v>16.14454721680685</v>
+        <v>22.16863645720131</v>
       </c>
       <c r="O4" t="n">
-        <v>15.36342304167505</v>
+        <v>21.38751228206951</v>
       </c>
       <c r="P4" t="n">
-        <v>0.1928113256989434</v>
+        <v>-0.9683815829837222</v>
       </c>
       <c r="Q4" t="n">
-        <v>3.295947110720648</v>
+        <v>8.464147581938811</v>
       </c>
       <c r="R4" t="n">
-        <v>45.56681417364126</v>
+        <v>15.63637601758669</v>
       </c>
       <c r="S4" t="n">
-        <v>6.157832711118325</v>
+        <v>4.424441548636277</v>
       </c>
       <c r="T4" t="n">
-        <v>16.31566542223665</v>
+        <v>12.84888309727255</v>
       </c>
       <c r="U4" t="n">
-        <v>15.53454124710485</v>
+        <v>12.06775892214075</v>
       </c>
       <c r="V4" t="n">
-        <v>0.4680455873035212</v>
+        <v>0.04131614060979941</v>
       </c>
       <c r="W4" t="n">
-        <v>0.02113752386723854</v>
+        <v>0.6124501621906998</v>
       </c>
       <c r="X4" t="n">
-        <v>2.94151114620424</v>
+        <v>2.014603288588439</v>
       </c>
       <c r="Y4" t="n">
-        <v>61.51347920053189</v>
+        <v>37.44135960423716</v>
       </c>
       <c r="Z4" t="n">
-        <v>3.922964562160437</v>
+        <v>1.740731709981168</v>
       </c>
       <c r="AA4" t="n">
-        <v>13.84592912432087</v>
+        <v>9.481463419962337</v>
       </c>
       <c r="AB4" t="n">
-        <v>12.67424286162317</v>
+        <v>8.309777157264636</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.7973904562220721</v>
+        <v>0.6228198800813587</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.9341101338713415</v>
+        <v>0.840203210487207</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.01365382168078832</v>
+        <v>0.5585799969912831</v>
       </c>
       <c r="AF4" t="n">
-        <v>0.919371145805998</v>
+        <v>0.6100055029598462</v>
       </c>
       <c r="AG4" t="n">
-        <v>2.910683944429047</v>
+        <v>1.623442592401094</v>
       </c>
       <c r="AH4" t="n">
-        <v>38.7993924961579</v>
+        <v>30.26285379069344</v>
       </c>
       <c r="AI4" t="n">
-        <v>2.024978517121248</v>
+        <v>1.887765611099858</v>
       </c>
       <c r="AJ4" t="n">
-        <v>14.0499570342425</v>
+        <v>13.77553122219971</v>
       </c>
       <c r="AK4" t="n">
-        <v>12.097146596413</v>
+        <v>11.82272078437021</v>
       </c>
       <c r="AL4" t="n">
-        <v>0.8086713969507556</v>
+        <v>0.5909607118143242</v>
       </c>
       <c r="AM4" t="n">
-        <v>0.8989465192670845</v>
+        <v>0.1055423671934228</v>
       </c>
       <c r="AN4" t="n">
-        <v>6.173037182225212</v>
+        <v>7.850907531614422</v>
       </c>
       <c r="AO4" t="n">
-        <v>62.69124900957895</v>
+        <v>64.46556015359562</v>
       </c>
       <c r="AP4" t="n">
-        <v>198.150351044467</v>
+        <v>180.3842851583507</v>
       </c>
       <c r="AQ4" t="n">
-        <v>6.002912784675861</v>
+        <v>4.295650127273347</v>
       </c>
       <c r="AR4" t="n">
-        <v>20.00582556935172</v>
+        <v>16.5913002545467</v>
       </c>
       <c r="AS4" t="n">
-        <v>18.44357721908812</v>
+        <v>15.0290519042831</v>
       </c>
       <c r="AT4" t="n">
-        <v>0.4776537334970183</v>
+        <v>0.06922254541395352</v>
       </c>
       <c r="AU4" t="n">
-        <v>0.4068993286275354</v>
+        <v>0.7081865861644375</v>
       </c>
       <c r="AV4" t="n">
-        <v>0.3184137264827819</v>
+        <v>0.5927208499153261</v>
       </c>
       <c r="AW4" t="n">
-        <v>6.079476793512687</v>
+        <v>8.175395749563554</v>
       </c>
       <c r="AX4" t="n">
-        <v>5.739640361965989</v>
+        <v>7.024531298238958</v>
       </c>
       <c r="AY4" t="n">
-        <v>42.310337083003</v>
+        <v>62.50725921398754</v>
       </c>
       <c r="AZ4" t="n">
-        <v>141.4138919786121</v>
+        <v>166.5115112349798</v>
       </c>
       <c r="BA4" t="n">
-        <v>98.96767077997565</v>
+        <v>130.6031530951853</v>
       </c>
       <c r="BB4" t="n">
-        <v>9.159825975026854</v>
+        <v>4.753211659364629</v>
       </c>
       <c r="BC4" t="n">
-        <v>32.3196519500537</v>
+        <v>23.50642331872926</v>
       </c>
       <c r="BD4" t="n">
-        <v>29.5857173370924</v>
+        <v>20.77248870576796</v>
       </c>
       <c r="BE4" t="n">
-        <v>-0.1806735902673747</v>
+        <v>-0.02992145969307939</v>
       </c>
       <c r="BF4" t="n">
-        <v>0.7698316337941457</v>
+        <v>0.2810324830063085</v>
       </c>
       <c r="BG4" t="n">
-        <v>1</v>
+        <v>9.340339051813697</v>
       </c>
       <c r="BH4" t="n">
-        <v>46.44128866441398</v>
+        <v>61.0668789408634</v>
       </c>
       <c r="BI4" t="n">
-        <v>0.4063922353009089</v>
+        <v>0.3542489822239152</v>
       </c>
       <c r="BJ4" t="n">
-        <v>0.254373264020427</v>
+        <v>10.44395963363118</v>
       </c>
       <c r="BK4" t="n">
-        <v>0.254373264020427</v>
+        <v>28.88791926726237</v>
       </c>
       <c r="BL4" t="n">
-        <v>18.70742389179658</v>
+        <v>27.32567091699876</v>
       </c>
       <c r="BM4" t="n">
-        <v>1.054525471885574</v>
+        <v>-1.262987411817226</v>
       </c>
       <c r="BN4" t="n">
-        <v>14.10905094377115</v>
+        <v>0.59519337407091</v>
       </c>
       <c r="BO4" t="n">
-        <v>11.76567841837575</v>
+        <v>1.940997198194067</v>
       </c>
       <c r="BP4" t="n">
-        <v>0.3866304377687335</v>
+        <v>41.10237644273074</v>
       </c>
       <c r="BQ4" t="n">
-        <v>15</v>
+        <v>0.530003178415769</v>
       </c>
       <c r="BR4" t="n">
-        <v>53.19177084440239</v>
+        <v>1.289770257597572</v>
       </c>
       <c r="BS4" t="n">
-        <v>0.8178130044598131</v>
+        <v>1.86138078289686</v>
       </c>
       <c r="BT4" t="n">
-        <v>3.358301295471719</v>
+        <v>13.72276156579372</v>
       </c>
       <c r="BU4" t="n">
-        <v>7.371457889722279</v>
+        <v>11.76995112796422</v>
       </c>
       <c r="BV4" t="n">
-        <v>24.74291577944456</v>
+        <v>0.5966777517283884</v>
       </c>
       <c r="BW4" t="n">
-        <v>22.79010534161506</v>
+        <v>1.254709370417751</v>
       </c>
       <c r="BX4" t="n">
-        <v>0.3014698361706379</v>
+        <v>50.68157108934793</v>
+      </c>
+      <c r="BY4" t="n">
+        <v>20.19514504044523</v>
+      </c>
+      <c r="BZ4" t="n">
+        <v>0.6657477210860696</v>
+      </c>
+      <c r="CA4" t="n">
+        <v>1.911901872779097</v>
+      </c>
+      <c r="CB4" t="n">
+        <v>11.82380374555819</v>
+      </c>
+      <c r="CC4" t="n">
+        <v>10.26155539529459</v>
+      </c>
+      <c r="CD4" t="n">
+        <v>0.5857308891929728</v>
+      </c>
+      <c r="CE4" t="n">
+        <v>9.43642544516973</v>
+      </c>
+      <c r="CF4" t="n">
+        <v>51.95545155875002</v>
+      </c>
+      <c r="CG4" t="n">
+        <v>54.57337685627155</v>
+      </c>
+      <c r="CH4" t="n">
+        <v>0.6373495095442747</v>
+      </c>
+      <c r="CI4" t="n">
+        <v>10.29377795448887</v>
+      </c>
+      <c r="CJ4" t="n">
+        <v>28.58755590897774</v>
+      </c>
+      <c r="CK4" t="n">
+        <v>27.02530755871414</v>
+      </c>
+      <c r="CL4" t="n">
+        <v>-1.230446185950149</v>
+      </c>
+      <c r="CM4" t="n">
+        <v>4.061905253857748</v>
+      </c>
+      <c r="CN4" t="n">
+        <v>33.05724778408902</v>
+      </c>
+      <c r="CO4" t="n">
+        <v>48.36700294147388</v>
+      </c>
+      <c r="CP4" t="n">
+        <v>0.2435092043633605</v>
+      </c>
+      <c r="CQ4" t="n">
+        <v>0.8137606733150059</v>
+      </c>
+      <c r="CR4" t="n">
+        <v>2.293150026302246</v>
+      </c>
+      <c r="CS4" t="n">
+        <v>14.58630005260449</v>
+      </c>
+      <c r="CT4" t="n">
+        <v>12.63348961477499</v>
+      </c>
+      <c r="CU4" t="n">
+        <v>0.5031223956266796</v>
       </c>
     </row>
     <row r="5">
@@ -1553,205 +1875,274 @@
         <v>10.83967894611662</v>
       </c>
       <c r="J5" t="n">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>48.6258650488428</v>
+        <v>65.94443553966529</v>
       </c>
       <c r="L5" t="n">
-        <v>7.55664315924962</v>
+        <v>1.697064829098816</v>
       </c>
       <c r="M5" t="n">
-        <v>10.49588908881453</v>
+        <v>8.399341584219137</v>
       </c>
       <c r="N5" t="n">
-        <v>24.99177817762906</v>
+        <v>20.79868316843827</v>
       </c>
       <c r="O5" t="n">
-        <v>24.21065400249726</v>
+        <v>20.01755899330648</v>
       </c>
       <c r="P5" t="n">
-        <v>0.4218532351856929</v>
+        <v>-0.8199614839024664</v>
       </c>
       <c r="Q5" t="n">
-        <v>6.202286100018399</v>
+        <v>3.706214204019247</v>
       </c>
       <c r="R5" t="n">
-        <v>35.27542411891869</v>
+        <v>41.2257318462835</v>
       </c>
       <c r="S5" t="n">
-        <v>3.94897668655767</v>
+        <v>3.083568151214604</v>
       </c>
       <c r="T5" t="n">
-        <v>11.89795337311534</v>
+        <v>10.16713630242921</v>
       </c>
       <c r="U5" t="n">
-        <v>11.11682919798354</v>
+        <v>9.386012127297407</v>
       </c>
       <c r="V5" t="n">
-        <v>0.6754048577975887</v>
+        <v>0.3318553350964062</v>
       </c>
       <c r="W5" t="n">
-        <v>0.5142758915209783</v>
+        <v>0.4180266776910356</v>
       </c>
       <c r="X5" t="n">
-        <v>8.243180885306716</v>
+        <v>1.715651990516265</v>
       </c>
       <c r="Y5" t="n">
-        <v>24.19557572868338</v>
+        <v>51.70974084656095</v>
       </c>
       <c r="Z5" t="n">
-        <v>2.719795723879855</v>
+        <v>1.448603985340918</v>
       </c>
       <c r="AA5" t="n">
-        <v>11.43959144775971</v>
+        <v>8.897207970681837</v>
       </c>
       <c r="AB5" t="n">
-        <v>10.26790518506201</v>
+        <v>7.725521707984139</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.3936335338102741</v>
+        <v>0.6861178424150035</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.2642861681726559</v>
+        <v>0.6563255861610752</v>
       </c>
       <c r="AE5" t="n">
-        <v>0.3935583591759801</v>
+        <v>0.2193199736765785</v>
       </c>
       <c r="AF5" t="n">
-        <v>0.5282505524756625</v>
+        <v>0.4432941885490438</v>
       </c>
       <c r="AG5" t="n">
-        <v>1.27626263755581</v>
+        <v>1.360555636053408</v>
       </c>
       <c r="AH5" t="n">
-        <v>47.68806534135416</v>
+        <v>56.27693091514785</v>
       </c>
       <c r="AI5" t="n">
-        <v>1.590562798808583</v>
+        <v>2.026895904010401</v>
       </c>
       <c r="AJ5" t="n">
-        <v>13.18112559761717</v>
+        <v>14.0537918080208</v>
       </c>
       <c r="AK5" t="n">
-        <v>11.22831515978767</v>
+        <v>12.1009813701913</v>
       </c>
       <c r="AL5" t="n">
-        <v>-0.03766692032708455</v>
+        <v>0.5608140899866089</v>
       </c>
       <c r="AM5" t="n">
+        <v>0.8584558778454271</v>
+      </c>
+      <c r="AN5" t="n">
+        <v>8.968256122318463</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>30.20590948971143</v>
+      </c>
+      <c r="AP5" t="n">
+        <v>191.0706495575795</v>
+      </c>
+      <c r="AQ5" t="n">
+        <v>3.32506693541836</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>14.65013387083672</v>
+      </c>
+      <c r="AS5" t="n">
+        <v>13.08788552057312</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>0.2795276042554691</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>0.5929236651192095</v>
+      </c>
+      <c r="AV5" t="n">
+        <v>0.5945243618375929</v>
+      </c>
+      <c r="AW5" t="n">
+        <v>5.506383012101076</v>
+      </c>
+      <c r="AX5" t="n">
+        <v>5.897212330106773</v>
+      </c>
+      <c r="AY5" t="n">
+        <v>77.64450079200851</v>
+      </c>
+      <c r="AZ5" t="n">
+        <v>67.25606884691562</v>
+      </c>
+      <c r="BA5" t="n">
+        <v>120.3135213646808</v>
+      </c>
+      <c r="BB5" t="n">
+        <v>5.383816482132853</v>
+      </c>
+      <c r="BC5" t="n">
+        <v>24.7676329642657</v>
+      </c>
+      <c r="BD5" t="n">
+        <v>22.03369835130441</v>
+      </c>
+      <c r="BE5" t="n">
+        <v>-0.1665603232865767</v>
+      </c>
+      <c r="BF5" t="n">
+        <v>0.02245109107207026</v>
+      </c>
+      <c r="BG5" t="n">
+        <v>2.137216848284956</v>
+      </c>
+      <c r="BH5" t="n">
+        <v>68.89984095597241</v>
+      </c>
+      <c r="BI5" t="n">
+        <v>0.515965373238379</v>
+      </c>
+      <c r="BJ5" t="n">
+        <v>2.850645397123813</v>
+      </c>
+      <c r="BK5" t="n">
+        <v>13.70129079424763</v>
+      </c>
+      <c r="BL5" t="n">
+        <v>12.13904244398403</v>
+      </c>
+      <c r="BM5" t="n">
+        <v>0.3823248197481767</v>
+      </c>
+      <c r="BN5" t="n">
+        <v>0.1046110538224809</v>
+      </c>
+      <c r="BO5" t="n">
+        <v>1.697069282074883</v>
+      </c>
+      <c r="BP5" t="n">
+        <v>65.04962121306112</v>
+      </c>
+      <c r="BQ5" t="n">
+        <v>0.9896854558299041</v>
+      </c>
+      <c r="BR5" t="n">
+        <v>1.60975811979622</v>
+      </c>
+      <c r="BS5" t="n">
+        <v>1.374436727944702</v>
+      </c>
+      <c r="BT5" t="n">
+        <v>12.7488734558894</v>
+      </c>
+      <c r="BU5" t="n">
+        <v>10.79606301805991</v>
+      </c>
+      <c r="BV5" t="n">
+        <v>0.7021883344261156</v>
+      </c>
+      <c r="BW5" t="n">
+        <v>4.408295825867963</v>
+      </c>
+      <c r="BX5" t="n">
+        <v>50.41046778381781</v>
+      </c>
+      <c r="BY5" t="n">
+        <v>44.47684417086404</v>
+      </c>
+      <c r="BZ5" t="n">
+        <v>0.4742453489771366</v>
+      </c>
+      <c r="CA5" t="n">
+        <v>3.124608981752625</v>
+      </c>
+      <c r="CB5" t="n">
+        <v>14.24921796350525</v>
+      </c>
+      <c r="CC5" t="n">
+        <v>12.68696961324165</v>
+      </c>
+      <c r="CD5" t="n">
+        <v>0.3229626462948338</v>
+      </c>
+      <c r="CE5" t="n">
+        <v>1.619062664535895</v>
+      </c>
+      <c r="CF5" t="n">
+        <v>41.73755813994335</v>
+      </c>
+      <c r="CG5" t="n">
+        <v>76.94941758968834</v>
+      </c>
+      <c r="CH5" t="n">
+        <v>0.3547406595972611</v>
+      </c>
+      <c r="CI5" t="n">
+        <v>1.63709566036468</v>
+      </c>
+      <c r="CJ5" t="n">
+        <v>11.27419132072936</v>
+      </c>
+      <c r="CK5" t="n">
+        <v>9.711942970465762</v>
+      </c>
+      <c r="CL5" t="n">
+        <v>0.645275642447326</v>
+      </c>
+      <c r="CM5" t="n">
         <v>1</v>
       </c>
-      <c r="AN5" t="n">
-        <v>10.31692527173229</v>
-      </c>
-      <c r="AO5" t="n">
-        <v>37.70574670503115</v>
-      </c>
-      <c r="AP5" t="n">
-        <v>144.6054267826657</v>
-      </c>
-      <c r="AQ5" t="n">
-        <v>6.295455703164067</v>
-      </c>
-      <c r="AR5" t="n">
-        <v>20.59091140632814</v>
-      </c>
-      <c r="AS5" t="n">
-        <v>19.02866305606453</v>
-      </c>
-      <c r="AT5" t="n">
-        <v>0.6982539743262056</v>
-      </c>
-      <c r="AU5" t="n">
-        <v>0.7056110439248885</v>
-      </c>
-      <c r="AV5" t="n">
-        <v>0.02456754469548237</v>
-      </c>
-      <c r="AW5" t="n">
-        <v>7.519136489596335</v>
-      </c>
-      <c r="AX5" t="n">
-        <v>10.94617171002813</v>
-      </c>
-      <c r="AY5" t="n">
-        <v>31.67041652905</v>
-      </c>
-      <c r="AZ5" t="n">
-        <v>72.05103179830611</v>
-      </c>
-      <c r="BA5" t="n">
-        <v>69.63214346853265</v>
-      </c>
-      <c r="BB5" t="n">
-        <v>3.184549675795648</v>
-      </c>
-      <c r="BC5" t="n">
-        <v>20.3690993515913</v>
-      </c>
-      <c r="BD5" t="n">
-        <v>17.63516473863</v>
-      </c>
-      <c r="BE5" t="n">
-        <v>0.6717282605715914</v>
-      </c>
-      <c r="BF5" t="n">
-        <v>0.6247176703506626</v>
-      </c>
-      <c r="BG5" t="n">
-        <v>10.33333333333333</v>
-      </c>
-      <c r="BH5" t="n">
-        <v>83.0333956568589</v>
-      </c>
-      <c r="BI5" t="n">
-        <v>0.4651037145848916</v>
-      </c>
-      <c r="BJ5" t="n">
-        <v>0.54553495858775</v>
-      </c>
-      <c r="BK5" t="n">
-        <v>0.54553495858775</v>
-      </c>
-      <c r="BL5" t="n">
-        <v>20.94217116881025</v>
-      </c>
-      <c r="BM5" t="n">
-        <v>3.372208831927177</v>
-      </c>
-      <c r="BN5" t="n">
-        <v>18.74441766385435</v>
-      </c>
-      <c r="BO5" t="n">
-        <v>16.40104513845895</v>
-      </c>
-      <c r="BP5" t="n">
-        <v>0.5542864547625208</v>
-      </c>
-      <c r="BQ5" t="n">
-        <v>11.2201389370414</v>
-      </c>
-      <c r="BR5" t="n">
-        <v>33.60973102079711</v>
-      </c>
-      <c r="BS5" t="n">
-        <v>0.8048702075134827</v>
-      </c>
-      <c r="BT5" t="n">
-        <v>3.575863947533554</v>
-      </c>
-      <c r="BU5" t="n">
-        <v>9.371048834715113</v>
-      </c>
-      <c r="BV5" t="n">
-        <v>28.74209766943023</v>
-      </c>
-      <c r="BW5" t="n">
-        <v>26.78928723160073</v>
-      </c>
-      <c r="BX5" t="n">
-        <v>-0.1856475925502468</v>
+      <c r="CN5" t="n">
+        <v>60.84869433057278</v>
+      </c>
+      <c r="CO5" t="n">
+        <v>60.40270944659761</v>
+      </c>
+      <c r="CP5" t="n">
+        <v>0.1031256453386403</v>
+      </c>
+      <c r="CQ5" t="n">
+        <v>0.1160387259418776</v>
+      </c>
+      <c r="CR5" t="n">
+        <v>4.007035401571467</v>
+      </c>
+      <c r="CS5" t="n">
+        <v>18.01407080314293</v>
+      </c>
+      <c r="CT5" t="n">
+        <v>16.06126036531343</v>
+      </c>
+      <c r="CU5" t="n">
+        <v>0.1317593144211077</v>
       </c>
     </row>
     <row r="6">
@@ -1789,205 +2180,274 @@
         <v>10.83967894611662</v>
       </c>
       <c r="J6" t="n">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>68.61111077354877</v>
+        <v>72.94443547225343</v>
       </c>
       <c r="L6" t="n">
-        <v>1</v>
+        <v>1.24907080247405</v>
       </c>
       <c r="M6" t="n">
-        <v>1.590234488127933</v>
+        <v>3.229571727892087</v>
       </c>
       <c r="N6" t="n">
-        <v>7.180468976255867</v>
+        <v>10.45914345578417</v>
       </c>
       <c r="O6" t="n">
-        <v>6.399344801124066</v>
+        <v>9.678019280652373</v>
       </c>
       <c r="P6" t="n">
-        <v>0.9119276951306051</v>
+        <v>0.3002194165662846</v>
       </c>
       <c r="Q6" t="n">
-        <v>2.205999430647057</v>
+        <v>5.956893672611888</v>
       </c>
       <c r="R6" t="n">
-        <v>33.30341388702567</v>
+        <v>62.25334581771236</v>
       </c>
       <c r="S6" t="n">
-        <v>1.898814960400647</v>
+        <v>2.746285594798293</v>
       </c>
       <c r="T6" t="n">
-        <v>7.797629920801294</v>
+        <v>9.492571189596587</v>
       </c>
       <c r="U6" t="n">
-        <v>7.016505745669494</v>
+        <v>8.711447014464786</v>
       </c>
       <c r="V6" t="n">
-        <v>0.7401267758721696</v>
+        <v>0.4049374041746711</v>
       </c>
       <c r="W6" t="n">
-        <v>0.02854146514956134</v>
+        <v>0.1648085154249241</v>
       </c>
       <c r="X6" t="n">
         <v>1</v>
       </c>
       <c r="Y6" t="n">
-        <v>68.2766670914334</v>
+        <v>72.78711847590201</v>
       </c>
       <c r="Z6" t="n">
-        <v>1.246019138856744</v>
+        <v>2.007552545032327</v>
       </c>
       <c r="AA6" t="n">
-        <v>8.492038277713489</v>
+        <v>10.01510509006466</v>
       </c>
       <c r="AB6" t="n">
-        <v>7.320352015015788</v>
+        <v>8.843418827366955</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.8831765857899327</v>
+        <v>0.5650053909304275</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.7019672803679189</v>
+        <v>0.3705826981981852</v>
       </c>
       <c r="AE6" t="n">
-        <v>0.004546270060736342</v>
+        <v>0.2977158999178095</v>
       </c>
       <c r="AF6" t="n">
-        <v>0.1800501856974492</v>
+        <v>0.4063422345413861</v>
       </c>
       <c r="AG6" t="n">
+        <v>1.029557832407198</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>56.18087593406919</v>
+      </c>
+      <c r="AI6" t="n">
+        <v>1.283860322601392</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>12.56772064520278</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>10.61491020737328</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>0.7218143452773562</v>
+      </c>
+      <c r="AM6" t="n">
+        <v>0.9963075791341715</v>
+      </c>
+      <c r="AN6" t="n">
+        <v>10</v>
+      </c>
+      <c r="AO6" t="n">
+        <v>35.37118394824672</v>
+      </c>
+      <c r="AP6" t="n">
+        <v>119.3582403316022</v>
+      </c>
+      <c r="AQ6" t="n">
+        <v>2.746610409350672</v>
+      </c>
+      <c r="AR6" t="n">
+        <v>13.49322081870135</v>
+      </c>
+      <c r="AS6" t="n">
+        <v>11.93097246843774</v>
+      </c>
+      <c r="AT6" t="n">
+        <v>0.4048670236610543</v>
+      </c>
+      <c r="AU6" t="n">
+        <v>0.7714095030733464</v>
+      </c>
+      <c r="AV6" t="n">
+        <v>0.2109666971267652</v>
+      </c>
+      <c r="AW6" t="n">
+        <v>7.287494085395241</v>
+      </c>
+      <c r="AX6" t="n">
+        <v>6.844306959731465</v>
+      </c>
+      <c r="AY6" t="n">
+        <v>47.75513254252049</v>
+      </c>
+      <c r="AZ6" t="n">
+        <v>105.3207351765223</v>
+      </c>
+      <c r="BA6" t="n">
+        <v>66.25844945111453</v>
+      </c>
+      <c r="BB6" t="n">
+        <v>3.171858151044224</v>
+      </c>
+      <c r="BC6" t="n">
+        <v>20.34371630208845</v>
+      </c>
+      <c r="BD6" t="n">
+        <v>17.60978168912715</v>
+      </c>
+      <c r="BE6" t="n">
+        <v>0.3127247404548498</v>
+      </c>
+      <c r="BF6" t="n">
+        <v>0.003669856924676456</v>
+      </c>
+      <c r="BG6" t="n">
+        <v>1.589632044157474</v>
+      </c>
+      <c r="BH6" t="n">
+        <v>73.71931495293072</v>
+      </c>
+      <c r="BI6" t="n">
+        <v>1.501156654050864</v>
+      </c>
+      <c r="BJ6" t="n">
+        <v>2.858747951601819</v>
+      </c>
+      <c r="BK6" t="n">
+        <v>13.71749590320364</v>
+      </c>
+      <c r="BL6" t="n">
+        <v>12.15524755294004</v>
+      </c>
+      <c r="BM6" t="n">
+        <v>0.3805691658170521</v>
+      </c>
+      <c r="BN6" t="n">
+        <v>0.08810833990768001</v>
+      </c>
+      <c r="BO6" t="n">
         <v>1</v>
       </c>
-      <c r="AH6" t="n">
-        <v>37.766451070486</v>
-      </c>
-      <c r="AI6" t="n">
-        <v>1.86757199556092</v>
-      </c>
-      <c r="AJ6" t="n">
-        <v>13.73514399112184</v>
-      </c>
-      <c r="AK6" t="n">
-        <v>11.78233355329234</v>
-      </c>
-      <c r="AL6" t="n">
-        <v>0.913131467676803</v>
-      </c>
-      <c r="AM6" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN6" t="n">
-        <v>7.33432412171209</v>
-      </c>
-      <c r="AO6" t="n">
-        <v>61.96037346070011</v>
-      </c>
-      <c r="AP6" t="n">
-        <v>200</v>
-      </c>
-      <c r="AQ6" t="n">
-        <v>1.981894781269511</v>
-      </c>
-      <c r="AR6" t="n">
-        <v>11.96378956253902</v>
-      </c>
-      <c r="AS6" t="n">
-        <v>10.40154121227542</v>
-      </c>
-      <c r="AT6" t="n">
-        <v>0.8104463989838703</v>
-      </c>
-      <c r="AU6" t="n">
-        <v>0.7550341640504441</v>
-      </c>
-      <c r="AV6" t="n">
-        <v>0.3977145470119544</v>
-      </c>
-      <c r="AW6" t="n">
-        <v>11.38660806672542</v>
-      </c>
-      <c r="AX6" t="n">
-        <v>1.644307478501329</v>
-      </c>
-      <c r="AY6" t="n">
-        <v>31.5425101996732</v>
-      </c>
-      <c r="AZ6" t="n">
-        <v>125.3044752606514</v>
-      </c>
-      <c r="BA6" t="n">
-        <v>96.87385990203158</v>
-      </c>
-      <c r="BB6" t="n">
-        <v>4.885351495093687</v>
-      </c>
-      <c r="BC6" t="n">
-        <v>23.77070299018737</v>
-      </c>
-      <c r="BD6" t="n">
-        <v>21.03676837722607</v>
-      </c>
-      <c r="BE6" t="n">
-        <v>0.4217948442883202</v>
-      </c>
-      <c r="BF6" t="n">
-        <v>0.5311110830127106</v>
-      </c>
-      <c r="BG6" t="n">
-        <v>5.666666666666667</v>
-      </c>
-      <c r="BH6" t="n">
-        <v>49.48524746820176</v>
-      </c>
-      <c r="BI6" t="n">
-        <v>0.4426398801754718</v>
-      </c>
-      <c r="BJ6" t="n">
-        <v>0.5043895094851316</v>
-      </c>
-      <c r="BK6" t="n">
-        <v>0.5043895094851316</v>
-      </c>
-      <c r="BL6" t="n">
-        <v>17.63057500108371</v>
-      </c>
-      <c r="BM6" t="n">
-        <v>2.155922437778923</v>
-      </c>
-      <c r="BN6" t="n">
-        <v>16.31184487555785</v>
-      </c>
-      <c r="BO6" t="n">
-        <v>13.96847235016245</v>
-      </c>
       <c r="BP6" t="n">
-        <v>0.8509125331394903</v>
+        <v>69.06637318497964</v>
       </c>
       <c r="BQ6" t="n">
-        <v>10.61667813105587</v>
+        <v>1.126848220510666</v>
       </c>
       <c r="BR6" t="n">
-        <v>65.97267748270136</v>
+        <v>1.725289336983161</v>
       </c>
       <c r="BS6" t="n">
-        <v>0.8390688485726567</v>
+        <v>0.9828631660448904</v>
       </c>
       <c r="BT6" t="n">
-        <v>3.684753972517293</v>
+        <v>11.96572633208978</v>
       </c>
       <c r="BU6" t="n">
-        <v>8.291633298507728</v>
+        <v>10.01291589426028</v>
       </c>
       <c r="BV6" t="n">
-        <v>26.58326659701546</v>
+        <v>0.7870341278286718</v>
       </c>
       <c r="BW6" t="n">
-        <v>24.63045615918596</v>
+        <v>1.349043752608271</v>
       </c>
       <c r="BX6" t="n">
-        <v>0.02585994667720297</v>
+        <v>75.45877466233706</v>
+      </c>
+      <c r="BY6" t="n">
+        <v>68.76786615363396</v>
+      </c>
+      <c r="BZ6" t="n">
+        <v>0.06189296929765608</v>
+      </c>
+      <c r="CA6" t="n">
+        <v>1.916137428915608</v>
+      </c>
+      <c r="CB6" t="n">
+        <v>11.83227485783121</v>
+      </c>
+      <c r="CC6" t="n">
+        <v>10.27002650756762</v>
+      </c>
+      <c r="CD6" t="n">
+        <v>0.5848131328481374</v>
+      </c>
+      <c r="CE6" t="n">
+        <v>1.24907466833868</v>
+      </c>
+      <c r="CF6" t="n">
+        <v>25.58895801374983</v>
+      </c>
+      <c r="CG6" t="n">
+        <v>72.94444260850305</v>
+      </c>
+      <c r="CH6" t="n">
+        <v>0</v>
+      </c>
+      <c r="CI6" t="n">
+        <v>3.229578316666749</v>
+      </c>
+      <c r="CJ6" t="n">
+        <v>14.4591566333335</v>
+      </c>
+      <c r="CK6" t="n">
+        <v>12.8969082830699</v>
+      </c>
+      <c r="CL6" t="n">
+        <v>0.3002179889167491</v>
+      </c>
+      <c r="CM6" t="n">
+        <v>4.84607194248874</v>
+      </c>
+      <c r="CN6" t="n">
+        <v>76.80306826421923</v>
+      </c>
+      <c r="CO6" t="n">
+        <v>53.88520473890836</v>
+      </c>
+      <c r="CP6" t="n">
+        <v>0.3060888880012875</v>
+      </c>
+      <c r="CQ6" t="n">
+        <v>0.4727551264696057</v>
+      </c>
+      <c r="CR6" t="n">
+        <v>2.379875573119771</v>
+      </c>
+      <c r="CS6" t="n">
+        <v>14.75975114623954</v>
+      </c>
+      <c r="CT6" t="n">
+        <v>12.80694070841004</v>
+      </c>
+      <c r="CU6" t="n">
+        <v>0.4843307852015453</v>
       </c>
     </row>
     <row r="7">
@@ -2025,205 +2485,274 @@
         <v>10.83967894611662</v>
       </c>
       <c r="J7" t="n">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>74.72221102185112</v>
+        <v>78.04731194708125</v>
       </c>
       <c r="L7" t="n">
-        <v>1.399889501679595</v>
+        <v>6.803816643430441</v>
       </c>
       <c r="M7" t="n">
-        <v>3.219498730570786</v>
+        <v>6.245190726688537</v>
       </c>
       <c r="N7" t="n">
-        <v>10.43899746114157</v>
+        <v>16.49038145337707</v>
       </c>
       <c r="O7" t="n">
-        <v>9.657873286009774</v>
+        <v>15.70925727824527</v>
       </c>
       <c r="P7" t="n">
-        <v>0.8495399441809361</v>
+        <v>-0.353202089501002</v>
       </c>
       <c r="Q7" t="n">
-        <v>2.018107361259708</v>
+        <v>7.43447110812455</v>
       </c>
       <c r="R7" t="n">
-        <v>51.55114352476686</v>
+        <v>20.67959664953017</v>
       </c>
       <c r="S7" t="n">
-        <v>2.457034217680067</v>
+        <v>4.451303145783331</v>
       </c>
       <c r="T7" t="n">
-        <v>8.914068435360134</v>
+        <v>12.90260629156666</v>
       </c>
       <c r="U7" t="n">
-        <v>8.132944260228333</v>
+        <v>12.12148211643486</v>
       </c>
       <c r="V7" t="n">
-        <v>0.7347301351908456</v>
+        <v>0.03549579484655582</v>
       </c>
       <c r="W7" t="n">
-        <v>0.1870594239245917</v>
+        <v>0.4852284616625939</v>
       </c>
       <c r="X7" t="n">
+        <v>2.14410272853622</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>46.4426108690187</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>8.713658677139403</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>23.4273173542788</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>22.25563109158111</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>-0.8880674178154111</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>0.9437660166306707</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>0.6068767105554078</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>0.8698167897779392</v>
+      </c>
+      <c r="AG7" t="n">
+        <v>1.617790323297173</v>
+      </c>
+      <c r="AH7" t="n">
+        <v>83.7390529968625</v>
+      </c>
+      <c r="AI7" t="n">
+        <v>2.074055604186278</v>
+      </c>
+      <c r="AJ7" t="n">
+        <v>14.14811120837255</v>
+      </c>
+      <c r="AK7" t="n">
+        <v>12.19530077054306</v>
+      </c>
+      <c r="AL7" t="n">
+        <v>0.5505955702309958</v>
+      </c>
+      <c r="AM7" t="n">
+        <v>0.4216761006699397</v>
+      </c>
+      <c r="AN7" t="n">
+        <v>9.381157631502003</v>
+      </c>
+      <c r="AO7" t="n">
+        <v>44.67426012035897</v>
+      </c>
+      <c r="AP7" t="n">
+        <v>125.5860843104078</v>
+      </c>
+      <c r="AQ7" t="n">
+        <v>4.775632232391264</v>
+      </c>
+      <c r="AR7" t="n">
+        <v>17.55126446478253</v>
+      </c>
+      <c r="AS7" t="n">
+        <v>15.98901611451893</v>
+      </c>
+      <c r="AT7" t="n">
+        <v>-0.03477952850077767</v>
+      </c>
+      <c r="AU7" t="n">
+        <v>0.865346580354892</v>
+      </c>
+      <c r="AV7" t="n">
+        <v>0.2451814084741339</v>
+      </c>
+      <c r="AW7" t="n">
+        <v>7.983141286979579</v>
+      </c>
+      <c r="AX7" t="n">
+        <v>7.066241217963563</v>
+      </c>
+      <c r="AY7" t="n">
+        <v>52.11648590338405</v>
+      </c>
+      <c r="AZ7" t="n">
+        <v>149.425515170554</v>
+      </c>
+      <c r="BA7" t="n">
+        <v>91.37203916436981</v>
+      </c>
+      <c r="BB7" t="n">
+        <v>2.114644934374727</v>
+      </c>
+      <c r="BC7" t="n">
+        <v>18.22928986874945</v>
+      </c>
+      <c r="BD7" t="n">
+        <v>15.49535525578816</v>
+      </c>
+      <c r="BE7" t="n">
+        <v>0.5418007121031675</v>
+      </c>
+      <c r="BF7" t="n">
+        <v>0.03717619794204811</v>
+      </c>
+      <c r="BG7" t="n">
+        <v>7.513549536313981</v>
+      </c>
+      <c r="BH7" t="n">
+        <v>73.71461674331555</v>
+      </c>
+      <c r="BI7" t="n">
+        <v>0.1567309447227921</v>
+      </c>
+      <c r="BJ7" t="n">
+        <v>9.090898057362628</v>
+      </c>
+      <c r="BK7" t="n">
+        <v>26.18179611472526</v>
+      </c>
+      <c r="BL7" t="n">
+        <v>24.61954776446166</v>
+      </c>
+      <c r="BM7" t="n">
+        <v>-0.9698072941299348</v>
+      </c>
+      <c r="BN7" t="n">
+        <v>0.5066964506816881</v>
+      </c>
+      <c r="BO7" t="n">
+        <v>4</v>
+      </c>
+      <c r="BP7" t="n">
+        <v>50.00508209830483</v>
+      </c>
+      <c r="BQ7" t="n">
+        <v>0.4119101922244107</v>
+      </c>
+      <c r="BR7" t="n">
+        <v>1.516455406010249</v>
+      </c>
+      <c r="BS7" t="n">
+        <v>2.580474633396096</v>
+      </c>
+      <c r="BT7" t="n">
+        <v>15.16094926679219</v>
+      </c>
+      <c r="BU7" t="n">
+        <v>13.20813882896269</v>
+      </c>
+      <c r="BV7" t="n">
+        <v>0.4408651683136852</v>
+      </c>
+      <c r="BW7" t="n">
         <v>1</v>
       </c>
-      <c r="Y7" t="n">
-        <v>75.09600714295128</v>
-      </c>
-      <c r="Z7" t="n">
-        <v>0.9569793322567647</v>
-      </c>
-      <c r="AA7" t="n">
-        <v>7.91395866451353</v>
-      </c>
-      <c r="AB7" t="n">
-        <v>6.742272401815829</v>
-      </c>
-      <c r="AC7" t="n">
-        <v>0.9200685697487415</v>
-      </c>
-      <c r="AD7" t="n">
-        <v>0.5539567514297054</v>
-      </c>
-      <c r="AE7" t="n">
-        <v>0.1743556467550783</v>
-      </c>
-      <c r="AF7" t="n">
-        <v>0.2554973171429886</v>
-      </c>
-      <c r="AG7" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH7" t="n">
-        <v>83.95237768491496</v>
-      </c>
-      <c r="AI7" t="n">
-        <v>0.9307549166339282</v>
-      </c>
-      <c r="AJ7" t="n">
-        <v>11.86150983326785</v>
-      </c>
-      <c r="AK7" t="n">
-        <v>9.908699395438358</v>
-      </c>
-      <c r="AL7" t="n">
-        <v>0.9203541025670553</v>
-      </c>
-      <c r="AM7" t="n">
-        <v>0.8302616379241846</v>
-      </c>
-      <c r="AN7" t="n">
-        <v>7.202144647009177</v>
-      </c>
-      <c r="AO7" t="n">
-        <v>19.94491041405561</v>
-      </c>
-      <c r="AP7" t="n">
-        <v>197.2078852545874</v>
-      </c>
-      <c r="AQ7" t="n">
-        <v>2.563301848019736</v>
-      </c>
-      <c r="AR7" t="n">
-        <v>13.12660369603947</v>
-      </c>
-      <c r="AS7" t="n">
-        <v>11.56435534577587</v>
-      </c>
-      <c r="AT7" t="n">
-        <v>0.7900742066275076</v>
-      </c>
-      <c r="AU7" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV7" t="n">
-        <v>0.2987080807729798</v>
-      </c>
-      <c r="AW7" t="n">
-        <v>14.00773920579197</v>
-      </c>
-      <c r="AX7" t="n">
-        <v>12.45892598600989</v>
-      </c>
-      <c r="AY7" t="n">
-        <v>62.92645561546123</v>
-      </c>
-      <c r="AZ7" t="n">
-        <v>167.1151652276474</v>
-      </c>
-      <c r="BA7" t="n">
-        <v>101.7875620168241</v>
-      </c>
-      <c r="BB7" t="n">
-        <v>4.688913831984249</v>
-      </c>
-      <c r="BC7" t="n">
-        <v>23.3778276639685</v>
-      </c>
-      <c r="BD7" t="n">
-        <v>20.6438930510072</v>
-      </c>
-      <c r="BE7" t="n">
-        <v>0.6809645975435495</v>
-      </c>
-      <c r="BF7" t="n">
-        <v>0.5881436235738823</v>
-      </c>
-      <c r="BG7" t="n">
-        <v>1.552510961700259</v>
-      </c>
-      <c r="BH7" t="n">
-        <v>44.50752229458581</v>
-      </c>
-      <c r="BI7" t="n">
-        <v>0.7414065893250795</v>
-      </c>
-      <c r="BJ7" t="n">
-        <v>0.2595696282601636</v>
-      </c>
-      <c r="BK7" t="n">
-        <v>0.2595696282601636</v>
-      </c>
-      <c r="BL7" t="n">
-        <v>7.968814382328458</v>
-      </c>
-      <c r="BM7" t="n">
-        <v>1.697006021857182</v>
-      </c>
-      <c r="BN7" t="n">
-        <v>15.39401204371436</v>
-      </c>
-      <c r="BO7" t="n">
-        <v>13.05063951831896</v>
-      </c>
-      <c r="BP7" t="n">
-        <v>0.7916760718377804</v>
-      </c>
-      <c r="BQ7" t="n">
-        <v>11.07496882189944</v>
-      </c>
-      <c r="BR7" t="n">
-        <v>37.03794343269384</v>
-      </c>
-      <c r="BS7" t="n">
-        <v>0.9287092826203184</v>
-      </c>
-      <c r="BT7" t="n">
-        <v>2.823186117216348</v>
-      </c>
-      <c r="BU7" t="n">
-        <v>8.644251602822848</v>
-      </c>
-      <c r="BV7" t="n">
-        <v>27.2885032056457</v>
-      </c>
-      <c r="BW7" t="n">
-        <v>25.3356927678162</v>
-      </c>
       <c r="BX7" t="n">
-        <v>-0.02231287012341439</v>
+        <v>63.19663870838119</v>
+      </c>
+      <c r="BY7" t="n">
+        <v>15.85175686113157</v>
+      </c>
+      <c r="BZ7" t="n">
+        <v>0.7276864752421529</v>
+      </c>
+      <c r="CA7" t="n">
+        <v>0.9898675907043621</v>
+      </c>
+      <c r="CB7" t="n">
+        <v>9.979735181408724</v>
+      </c>
+      <c r="CC7" t="n">
+        <v>8.417486831145126</v>
+      </c>
+      <c r="CD7" t="n">
+        <v>0.7855164156402442</v>
+      </c>
+      <c r="CE7" t="n">
+        <v>9.340894250247798</v>
+      </c>
+      <c r="CF7" t="n">
+        <v>35.41044695283639</v>
+      </c>
+      <c r="CG7" t="n">
+        <v>53.90268311424192</v>
+      </c>
+      <c r="CH7" t="n">
+        <v>0.5379965223946249</v>
+      </c>
+      <c r="CI7" t="n">
+        <v>10.53465082410505</v>
+      </c>
+      <c r="CJ7" t="n">
+        <v>29.0693016482101</v>
+      </c>
+      <c r="CK7" t="n">
+        <v>27.5070532979465</v>
+      </c>
+      <c r="CL7" t="n">
+        <v>-1.28263829420327</v>
+      </c>
+      <c r="CM7" t="n">
+        <v>4</v>
+      </c>
+      <c r="CN7" t="n">
+        <v>58.11836337262091</v>
+      </c>
+      <c r="CO7" t="n">
+        <v>36.60996122614728</v>
+      </c>
+      <c r="CP7" t="n">
+        <v>0.2357091957195004</v>
+      </c>
+      <c r="CQ7" t="n">
+        <v>0.6449772309446603</v>
+      </c>
+      <c r="CR7" t="n">
+        <v>1.849688870313286</v>
+      </c>
+      <c r="CS7" t="n">
+        <v>13.69937774062657</v>
+      </c>
+      <c r="CT7" t="n">
+        <v>11.74656730279707</v>
+      </c>
+      <c r="CU7" t="n">
+        <v>0.5992111444189817</v>
       </c>
     </row>
     <row r="8">
@@ -2240,7 +2769,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>rwpd</t>
+          <t>rwp</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -2261,205 +2790,274 @@
         <v>10.83967894611662</v>
       </c>
       <c r="J8" t="n">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="K8" t="n">
-        <v>48.0344744235295</v>
+        <v>62.61109580559609</v>
       </c>
       <c r="L8" t="n">
-        <v>9.052881411170887</v>
+        <v>2.393941178662079</v>
       </c>
       <c r="M8" t="n">
-        <v>11.32142224999441</v>
+        <v>8.023152716516575</v>
       </c>
       <c r="N8" t="n">
-        <v>26.64284449998882</v>
+        <v>20.04630543303315</v>
       </c>
       <c r="O8" t="n">
-        <v>25.86172032485702</v>
+        <v>19.26518125790136</v>
       </c>
       <c r="P8" t="n">
-        <v>-0.1806493080710839</v>
+        <v>-0.7384492316590437</v>
       </c>
       <c r="Q8" t="n">
-        <v>15</v>
+        <v>6.008002702358648</v>
       </c>
       <c r="R8" t="n">
-        <v>54.4300685541291</v>
+        <v>32.22411271140535</v>
       </c>
       <c r="S8" t="n">
-        <v>4.061901096741779</v>
+        <v>3.027706251184277</v>
       </c>
       <c r="T8" t="n">
-        <v>12.12380219348356</v>
+        <v>10.05541250236855</v>
       </c>
       <c r="U8" t="n">
-        <v>11.34267801835176</v>
+        <v>9.274288327236754</v>
       </c>
       <c r="V8" t="n">
-        <v>0.2753794361774598</v>
+        <v>0.3439594393828445</v>
       </c>
       <c r="W8" t="n">
-        <v>0.3535440692784063</v>
+        <v>0.09950168957932488</v>
       </c>
       <c r="X8" t="n">
-        <v>7.514259562800888</v>
+        <v>2.6925788384354</v>
       </c>
       <c r="Y8" t="n">
-        <v>28.88654057476038</v>
+        <v>53.03896127999108</v>
       </c>
       <c r="Z8" t="n">
-        <v>11.26368041600993</v>
+        <v>4.082881312628359</v>
       </c>
       <c r="AA8" t="n">
-        <v>28.52736083201986</v>
+        <v>14.16576262525672</v>
       </c>
       <c r="AB8" t="n">
-        <v>27.35567456932215</v>
+        <v>12.99407636255902</v>
       </c>
       <c r="AC8" t="n">
-        <v>0.1482116048741078</v>
+        <v>0.1153250933037784</v>
       </c>
       <c r="AD8" t="n">
-        <v>0.04276248893648877</v>
+        <v>0.7855185398806611</v>
       </c>
       <c r="AE8" t="n">
-        <v>0.08204889969164979</v>
+        <v>0.1773029132643072</v>
       </c>
       <c r="AF8" t="n">
-        <v>0.6130830130051196</v>
+        <v>0.7345270167314483</v>
       </c>
       <c r="AG8" t="n">
-        <v>7.762115881123101</v>
+        <v>3.562074558238146</v>
       </c>
       <c r="AH8" t="n">
-        <v>3.945781687537985</v>
+        <v>68.33654665286488</v>
       </c>
       <c r="AI8" t="n">
-        <v>10.65412043780244</v>
+        <v>3.262956295870717</v>
       </c>
       <c r="AJ8" t="n">
-        <v>31.30824087560487</v>
+        <v>16.52591259174143</v>
       </c>
       <c r="AK8" t="n">
-        <v>29.35543043777537</v>
+        <v>14.57310215391193</v>
       </c>
       <c r="AL8" t="n">
-        <v>0.7483594888682822</v>
+        <v>0.2929856795800446</v>
       </c>
       <c r="AM8" t="n">
-        <v>0.3108121937196251</v>
+        <v>1</v>
       </c>
       <c r="AN8" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="AO8" t="n">
-        <v>55.24827298506117</v>
+        <v>83.57808566478556</v>
       </c>
       <c r="AP8" t="n">
-        <v>44.0504548528347</v>
+        <v>105.1230510651738</v>
       </c>
       <c r="AQ8" t="n">
-        <v>4.933240682252332</v>
+        <v>3.142255627636481</v>
       </c>
       <c r="AR8" t="n">
-        <v>17.86648136450467</v>
+        <v>14.28451125527296</v>
       </c>
       <c r="AS8" t="n">
-        <v>16.30423301424107</v>
+        <v>12.72226290500936</v>
       </c>
       <c r="AT8" t="n">
-        <v>0.6068810816519923</v>
+        <v>0.3191389875584129</v>
       </c>
       <c r="AU8" t="n">
-        <v>0.1196237470882067</v>
+        <v>0.6977961475473374</v>
       </c>
       <c r="AV8" t="n">
-        <v>0.3171912307106964</v>
+        <v>0.8439733667961438</v>
       </c>
       <c r="AW8" t="n">
-        <v>7.018576866239161</v>
+        <v>5.238515798723514</v>
       </c>
       <c r="AX8" t="n">
-        <v>10.91455327359442</v>
+        <v>6.817869421660068</v>
       </c>
       <c r="AY8" t="n">
-        <v>37.60938931393168</v>
+        <v>78.32130095399692</v>
       </c>
       <c r="AZ8" t="n">
-        <v>89.72400759586951</v>
+        <v>73.75251850107566</v>
       </c>
       <c r="BA8" t="n">
-        <v>163.9748437878742</v>
+        <v>79.62694527460613</v>
       </c>
       <c r="BB8" t="n">
-        <v>8.321127711755727</v>
+        <v>5.526006274296202</v>
       </c>
       <c r="BC8" t="n">
-        <v>30.64225542351145</v>
+        <v>25.0520125485924</v>
       </c>
       <c r="BD8" t="n">
-        <v>27.90832081055015</v>
+        <v>22.31807793563111</v>
       </c>
       <c r="BE8" t="n">
-        <v>0.7282469234871239</v>
+        <v>-0.1973698745527847</v>
       </c>
       <c r="BF8" t="n">
-        <v>0.334389636380622</v>
+        <v>0.05824930926367844</v>
       </c>
       <c r="BG8" t="n">
-        <v>7.962386049300626</v>
+        <v>2.563602873621116</v>
       </c>
       <c r="BH8" t="n">
-        <v>37.67476568664516</v>
+        <v>70.05040178184511</v>
       </c>
       <c r="BI8" t="n">
-        <v>0.2787855443169838</v>
+        <v>1.472839654334117</v>
       </c>
       <c r="BJ8" t="n">
-        <v>0.2139453119199318</v>
+        <v>1.89795791033573</v>
       </c>
       <c r="BK8" t="n">
-        <v>0.2139453119199318</v>
+        <v>11.79591582067146</v>
       </c>
       <c r="BL8" t="n">
-        <v>4.006273736558172</v>
+        <v>10.23366747040786</v>
       </c>
       <c r="BM8" t="n">
-        <v>3.612160570921269</v>
+        <v>0.5887522539422753</v>
       </c>
       <c r="BN8" t="n">
-        <v>19.22432114184254</v>
+        <v>0.07692620103541079</v>
       </c>
       <c r="BO8" t="n">
-        <v>16.88094861644714</v>
+        <v>1</v>
       </c>
       <c r="BP8" t="n">
-        <v>0.384081049562534</v>
+        <v>67.80283874718693</v>
       </c>
       <c r="BQ8" t="n">
-        <v>1.946427299139617</v>
+        <v>1.204989361710195</v>
       </c>
       <c r="BR8" t="n">
-        <v>43.23369741156737</v>
+        <v>0.4046966747409677</v>
       </c>
       <c r="BS8" t="n">
-        <v>0.6487981679185917</v>
+        <v>0.9707646233344365</v>
       </c>
       <c r="BT8" t="n">
-        <v>3.401351218508614</v>
+        <v>11.94152924666887</v>
       </c>
       <c r="BU8" t="n">
-        <v>1.640958273078826</v>
+        <v>9.988718808839375</v>
       </c>
       <c r="BV8" t="n">
-        <v>13.28191654615765</v>
+        <v>0.7896556287550949</v>
       </c>
       <c r="BW8" t="n">
-        <v>11.32910610832815</v>
+        <v>7.141461619657668</v>
       </c>
       <c r="BX8" t="n">
-        <v>0.2338406076765422</v>
+        <v>28.91903679666373</v>
+      </c>
+      <c r="BY8" t="n">
+        <v>65.24742560795742</v>
+      </c>
+      <c r="BZ8" t="n">
+        <v>0.2685705646636552</v>
+      </c>
+      <c r="CA8" t="n">
+        <v>6.596098469346356</v>
+      </c>
+      <c r="CB8" t="n">
+        <v>21.19219693869271</v>
+      </c>
+      <c r="CC8" t="n">
+        <v>19.62994858842911</v>
+      </c>
+      <c r="CD8" t="n">
+        <v>-0.4292364511990996</v>
+      </c>
+      <c r="CE8" t="n">
+        <v>3.022265951882081</v>
+      </c>
+      <c r="CF8" t="n">
+        <v>41.94197958130525</v>
+      </c>
+      <c r="CG8" t="n">
+        <v>68.02532641720207</v>
+      </c>
+      <c r="CH8" t="n">
+        <v>0.2401837940924735</v>
+      </c>
+      <c r="CI8" t="n">
+        <v>2.598020773069728</v>
+      </c>
+      <c r="CJ8" t="n">
+        <v>13.19604154613946</v>
+      </c>
+      <c r="CK8" t="n">
+        <v>11.63379319587586</v>
+      </c>
+      <c r="CL8" t="n">
+        <v>0.4370632871689559</v>
+      </c>
+      <c r="CM8" t="n">
+        <v>1</v>
+      </c>
+      <c r="CN8" t="n">
+        <v>14.76555240046555</v>
+      </c>
+      <c r="CO8" t="n">
+        <v>47.33862686641752</v>
+      </c>
+      <c r="CP8" t="n">
+        <v>0.3842541094366119</v>
+      </c>
+      <c r="CQ8" t="n">
+        <v>0.3320702188579819</v>
+      </c>
+      <c r="CR8" t="n">
+        <v>1.610474522068065</v>
+      </c>
+      <c r="CS8" t="n">
+        <v>13.22094904413613</v>
+      </c>
+      <c r="CT8" t="n">
+        <v>11.26813860630663</v>
+      </c>
+      <c r="CU8" t="n">
+        <v>0.6510438858116047</v>
       </c>
     </row>
     <row r="9">
@@ -2476,7 +3074,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>rwp</t>
+          <t>rwfp</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -2497,205 +3095,1189 @@
         <v>10.83967894611662</v>
       </c>
       <c r="J9" t="n">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>25.08559276623879</v>
+        <v>20.29686392988893</v>
       </c>
       <c r="L9" t="n">
-        <v>6.959270348932836</v>
+        <v>7.567641098474051</v>
       </c>
       <c r="M9" t="n">
-        <v>9.658636519244411</v>
+        <v>4.099250274089193</v>
       </c>
       <c r="N9" t="n">
-        <v>23.31727303848882</v>
+        <v>12.19850054817839</v>
       </c>
       <c r="O9" t="n">
-        <v>22.53614886335702</v>
+        <v>11.41737637304658</v>
       </c>
       <c r="P9" t="n">
-        <v>0.4112979575360707</v>
+        <v>0.1117782820339318</v>
       </c>
       <c r="Q9" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="R9" t="n">
-        <v>72.80625173226349</v>
+        <v>55.94473021950392</v>
       </c>
       <c r="S9" t="n">
-        <v>3.829363654257641</v>
+        <v>3.547638561482741</v>
       </c>
       <c r="T9" t="n">
-        <v>11.65872730851528</v>
+        <v>11.09527712296548</v>
       </c>
       <c r="U9" t="n">
-        <v>10.87760313338348</v>
+        <v>10.31415294783368</v>
       </c>
       <c r="V9" t="n">
-        <v>0.6067365335081214</v>
+        <v>0.2313009923496296</v>
       </c>
       <c r="W9" t="n">
-        <v>0.07099203562612018</v>
+        <v>0.0183387811710823</v>
       </c>
       <c r="X9" t="n">
-        <v>8.765646709289188</v>
+        <v>7.964653821735588</v>
       </c>
       <c r="Y9" t="n">
-        <v>28.6274554129281</v>
+        <v>18.818296436243</v>
       </c>
       <c r="Z9" t="n">
-        <v>5.87678179119392</v>
+        <v>4.469843804982864</v>
       </c>
       <c r="AA9" t="n">
-        <v>17.75356358238784</v>
+        <v>14.93968760996573</v>
       </c>
       <c r="AB9" t="n">
-        <v>16.58187731969014</v>
+        <v>13.76800134726803</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.4001248224085712</v>
+        <v>0.03147842214049656</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.4328589680918574</v>
+        <v>0.4245221274913454</v>
       </c>
       <c r="AE9" t="n">
-        <v>0.01448960918412934</v>
+        <v>0.01650754483057411</v>
       </c>
       <c r="AF9" t="n">
-        <v>0.1079385057113843</v>
+        <v>0.2258096594879324</v>
       </c>
       <c r="AG9" t="n">
-        <v>7.468647125816472</v>
+        <v>10</v>
       </c>
       <c r="AH9" t="n">
-        <v>14.7797885236327</v>
+        <v>45.61394579355905</v>
       </c>
       <c r="AI9" t="n">
-        <v>5.306539799353574</v>
+        <v>10.72954252727119</v>
       </c>
       <c r="AJ9" t="n">
-        <v>20.61307959870715</v>
+        <v>31.45908505454237</v>
       </c>
       <c r="AK9" t="n">
-        <v>18.66026916087765</v>
+        <v>29.50627461671288</v>
       </c>
       <c r="AL9" t="n">
-        <v>0.704293661887383</v>
+        <v>-1.32486724628696</v>
       </c>
       <c r="AM9" t="n">
         <v>0.3333333333333333</v>
       </c>
       <c r="AN9" t="n">
-        <v>15</v>
+        <v>9.019920584524003</v>
       </c>
       <c r="AO9" t="n">
-        <v>52.83105880366109</v>
+        <v>36.60053612092904</v>
       </c>
       <c r="AP9" t="n">
-        <v>44.89872185382453</v>
+        <v>40.6848761367846</v>
       </c>
       <c r="AQ9" t="n">
-        <v>4.402068261548706</v>
+        <v>4.463826530688807</v>
       </c>
       <c r="AR9" t="n">
-        <v>16.80413652309741</v>
+        <v>16.92765306137762</v>
       </c>
       <c r="AS9" t="n">
-        <v>15.24188817283381</v>
+        <v>15.36540471111402</v>
       </c>
       <c r="AT9" t="n">
-        <v>0.6062360522756007</v>
+        <v>0.0327822395104003</v>
       </c>
       <c r="AU9" t="n">
-        <v>0.5384495480707577</v>
+        <v>0.4868400545286831</v>
       </c>
       <c r="AV9" t="n">
-        <v>0.03527561726336065</v>
+        <v>0.6891867076734739</v>
       </c>
       <c r="AW9" t="n">
-        <v>5.96076506955588</v>
+        <v>5.155265892918218</v>
       </c>
       <c r="AX9" t="n">
-        <v>10.99962875470725</v>
+        <v>4.242331926492202</v>
       </c>
       <c r="AY9" t="n">
-        <v>75.41472869700061</v>
+        <v>68.86947116454509</v>
       </c>
       <c r="AZ9" t="n">
-        <v>79.05514161990187</v>
+        <v>128.3934191486618</v>
       </c>
       <c r="BA9" t="n">
-        <v>103.3767965057558</v>
+        <v>160.1544651557397</v>
       </c>
       <c r="BB9" t="n">
-        <v>11.0102729827281</v>
+        <v>9.716977921732127</v>
       </c>
       <c r="BC9" t="n">
-        <v>36.0205459654562</v>
+        <v>33.43395584346425</v>
       </c>
       <c r="BD9" t="n">
-        <v>33.28661135249489</v>
+        <v>30.70002123050295</v>
       </c>
       <c r="BE9" t="n">
-        <v>0.3619237751571194</v>
+        <v>-1.105465693966914</v>
       </c>
       <c r="BF9" t="n">
-        <v>0.668039044325018</v>
+        <v>0.5018509714120291</v>
       </c>
       <c r="BG9" t="n">
-        <v>6.988588322006115</v>
+        <v>6.465226730206865</v>
       </c>
       <c r="BH9" t="n">
-        <v>50.90438144327169</v>
+        <v>45.33626950141008</v>
       </c>
       <c r="BI9" t="n">
-        <v>0.3157129234519341</v>
+        <v>0.7177044604255939</v>
       </c>
       <c r="BJ9" t="n">
-        <v>0.4591704831257128</v>
+        <v>2.562308246828959</v>
       </c>
       <c r="BK9" t="n">
-        <v>0.4591704831257128</v>
+        <v>13.12461649365792</v>
       </c>
       <c r="BL9" t="n">
-        <v>7.618451480689317</v>
+        <v>11.56236814339432</v>
       </c>
       <c r="BM9" t="n">
-        <v>7.090992919741713</v>
+        <v>0.4448014439755763</v>
       </c>
       <c r="BN9" t="n">
-        <v>26.18198583948343</v>
+        <v>0.7030720577724635</v>
       </c>
       <c r="BO9" t="n">
-        <v>23.83861331408803</v>
+        <v>5.459422729826336</v>
       </c>
       <c r="BP9" t="n">
-        <v>0.713023495510588</v>
+        <v>66.42630653965706</v>
       </c>
       <c r="BQ9" t="n">
-        <v>13.66749950831805</v>
+        <v>1.791863587570441</v>
       </c>
       <c r="BR9" t="n">
-        <v>57.99057806472572</v>
+        <v>0.3235063334496823</v>
       </c>
       <c r="BS9" t="n">
-        <v>0.6375751195359797</v>
+        <v>2.801889294356442</v>
       </c>
       <c r="BT9" t="n">
-        <v>2.136118951813969</v>
+        <v>15.60377858871288</v>
       </c>
       <c r="BU9" t="n">
-        <v>4.177437017562668</v>
+        <v>13.65096815088339</v>
       </c>
       <c r="BV9" t="n">
-        <v>18.35487403512534</v>
+        <v>0.3928892465252136</v>
       </c>
       <c r="BW9" t="n">
-        <v>16.40206359729584</v>
+        <v>9.206922833302075</v>
       </c>
       <c r="BX9" t="n">
-        <v>0.5222586853689359</v>
+        <v>47.20370439830373</v>
+      </c>
+      <c r="BY9" t="n">
+        <v>34.30926301205407</v>
+      </c>
+      <c r="BZ9" t="n">
+        <v>0.007083050527783936</v>
+      </c>
+      <c r="CA9" t="n">
+        <v>10.37155175143288</v>
+      </c>
+      <c r="CB9" t="n">
+        <v>28.74310350286575</v>
+      </c>
+      <c r="CC9" t="n">
+        <v>27.18085515260215</v>
+      </c>
+      <c r="CD9" t="n">
+        <v>-1.247298139579572</v>
+      </c>
+      <c r="CE9" t="n">
+        <v>5.583633008752144</v>
+      </c>
+      <c r="CF9" t="n">
+        <v>45.09736951696615</v>
+      </c>
+      <c r="CG9" t="n">
+        <v>55.36497966704363</v>
+      </c>
+      <c r="CH9" t="n">
+        <v>1.696165742564435</v>
+      </c>
+      <c r="CI9" t="n">
+        <v>2.24468490201637</v>
+      </c>
+      <c r="CJ9" t="n">
+        <v>12.48936980403274</v>
+      </c>
+      <c r="CK9" t="n">
+        <v>10.92712145376914</v>
+      </c>
+      <c r="CL9" t="n">
+        <v>0.5136237734583134</v>
+      </c>
+      <c r="CM9" t="n">
+        <v>7</v>
+      </c>
+      <c r="CN9" t="n">
+        <v>35.82446969272163</v>
+      </c>
+      <c r="CO9" t="n">
+        <v>11.04282668616817</v>
+      </c>
+      <c r="CP9" t="n">
+        <v>0.6095479370331452</v>
+      </c>
+      <c r="CQ9" t="n">
+        <v>0.09591675297084584</v>
+      </c>
+      <c r="CR9" t="n">
+        <v>2.423641161932785</v>
+      </c>
+      <c r="CS9" t="n">
+        <v>14.84728232386557</v>
+      </c>
+      <c r="CT9" t="n">
+        <v>12.89447188603607</v>
+      </c>
+      <c r="CU9" t="n">
+        <v>0.4748476983236822</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>5c884b29c2ceec001719b1e4</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>lmf</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>neut</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>5</v>
+      </c>
+      <c r="G10" t="n">
+        <v>4.61512051684126</v>
+      </c>
+      <c r="H10" t="n">
+        <v>11.23024103368252</v>
+      </c>
+      <c r="I10" t="n">
+        <v>10.83967894611662</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>24.3888887511591</v>
+      </c>
+      <c r="L10" t="n">
+        <v>1</v>
+      </c>
+      <c r="M10" t="n">
+        <v>1.201345788883664</v>
+      </c>
+      <c r="N10" t="n">
+        <v>6.402691577767327</v>
+      </c>
+      <c r="O10" t="n">
+        <v>5.621567402635527</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.7396935173199108</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>1.705760613150595</v>
+      </c>
+      <c r="R10" t="n">
+        <v>83.57122982366984</v>
+      </c>
+      <c r="S10" t="n">
+        <v>1.481743624787051</v>
+      </c>
+      <c r="T10" t="n">
+        <v>6.963487249574101</v>
+      </c>
+      <c r="U10" t="n">
+        <v>6.182363074442303</v>
+      </c>
+      <c r="V10" t="n">
+        <v>0.6789371763142591</v>
+      </c>
+      <c r="W10" t="n">
+        <v>0.01018749730572943</v>
+      </c>
+      <c r="X10" t="n">
+        <v>1.056061277262186</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>23.77518155477219</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>1.157267266881945</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>8.31453453376389</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>7.14284827106619</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>0.7492444102686148</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>0.3001897653965162</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>0.01447953108444827</v>
+      </c>
+      <c r="AF10" t="n">
+        <v>0.3156114605358817</v>
+      </c>
+      <c r="AG10" t="n">
+        <v>1.303781486420566</v>
+      </c>
+      <c r="AH10" t="n">
+        <v>3.882019416997946</v>
+      </c>
+      <c r="AI10" t="n">
+        <v>1.835146686607677</v>
+      </c>
+      <c r="AJ10" t="n">
+        <v>13.67029337321535</v>
+      </c>
+      <c r="AK10" t="n">
+        <v>11.71748293538585</v>
+      </c>
+      <c r="AL10" t="n">
+        <v>0.6023621311922508</v>
+      </c>
+      <c r="AM10" t="n">
+        <v>0.1526713754701107</v>
+      </c>
+      <c r="AN10" t="n">
+        <v>4.583114660274119</v>
+      </c>
+      <c r="AO10" t="n">
+        <v>55.08016031253778</v>
+      </c>
+      <c r="AP10" t="n">
+        <v>94.55117977166394</v>
+      </c>
+      <c r="AQ10" t="n">
+        <v>2.239599255516187</v>
+      </c>
+      <c r="AR10" t="n">
+        <v>12.47919851103237</v>
+      </c>
+      <c r="AS10" t="n">
+        <v>10.91695016076878</v>
+      </c>
+      <c r="AT10" t="n">
+        <v>0.5147257265885999</v>
+      </c>
+      <c r="AU10" t="n">
+        <v>0.3467972772786215</v>
+      </c>
+      <c r="AV10" t="n">
+        <v>0.1951612922185138</v>
+      </c>
+      <c r="AW10" t="n">
+        <v>9.226591941896428</v>
+      </c>
+      <c r="AX10" t="n">
+        <v>4.403463364451361</v>
+      </c>
+      <c r="AY10" t="n">
+        <v>86.29737996987031</v>
+      </c>
+      <c r="AZ10" t="n">
+        <v>108.0875035427641</v>
+      </c>
+      <c r="BA10" t="n">
+        <v>113.8801215202933</v>
+      </c>
+      <c r="BB10" t="n">
+        <v>8.879705411208858</v>
+      </c>
+      <c r="BC10" t="n">
+        <v>31.75941082241772</v>
+      </c>
+      <c r="BD10" t="n">
+        <v>29.02547620945642</v>
+      </c>
+      <c r="BE10" t="n">
+        <v>-0.9240462689555983</v>
+      </c>
+      <c r="BF10" t="n">
+        <v>0.3219289477497752</v>
+      </c>
+      <c r="BG10" t="n">
+        <v>4</v>
+      </c>
+      <c r="BH10" t="n">
+        <v>24.42040027750089</v>
+      </c>
+      <c r="BI10" t="n">
+        <v>1.674106790196913</v>
+      </c>
+      <c r="BJ10" t="n">
+        <v>2.62586477126788</v>
+      </c>
+      <c r="BK10" t="n">
+        <v>13.25172954253576</v>
+      </c>
+      <c r="BL10" t="n">
+        <v>11.68948119227216</v>
+      </c>
+      <c r="BM10" t="n">
+        <v>0.431030075664176</v>
+      </c>
+      <c r="BN10" t="n">
+        <v>0.01355931631105856</v>
+      </c>
+      <c r="BO10" t="n">
+        <v>1</v>
+      </c>
+      <c r="BP10" t="n">
+        <v>23.46679810654935</v>
+      </c>
+      <c r="BQ10" t="n">
+        <v>0.3299700139498863</v>
+      </c>
+      <c r="BR10" t="n">
+        <v>1.071659709856087</v>
+      </c>
+      <c r="BS10" t="n">
+        <v>1.018362681659006</v>
+      </c>
+      <c r="BT10" t="n">
+        <v>12.03672536331801</v>
+      </c>
+      <c r="BU10" t="n">
+        <v>10.08391492548851</v>
+      </c>
+      <c r="BV10" t="n">
+        <v>0.779342125965541</v>
+      </c>
+      <c r="BW10" t="n">
+        <v>1</v>
+      </c>
+      <c r="BX10" t="n">
+        <v>35.77730075362717</v>
+      </c>
+      <c r="BY10" t="n">
+        <v>23.06176420436623</v>
+      </c>
+      <c r="BZ10" t="n">
+        <v>0.01674879550935695</v>
+      </c>
+      <c r="CA10" t="n">
+        <v>1.588033808863957</v>
+      </c>
+      <c r="CB10" t="n">
+        <v>11.17606761772791</v>
+      </c>
+      <c r="CC10" t="n">
+        <v>9.613819267464315</v>
+      </c>
+      <c r="CD10" t="n">
+        <v>0.6559063185741334</v>
+      </c>
+      <c r="CE10" t="n">
+        <v>1</v>
+      </c>
+      <c r="CF10" t="n">
+        <v>52.12253282603837</v>
+      </c>
+      <c r="CG10" t="n">
+        <v>24.72905413510719</v>
+      </c>
+      <c r="CH10" t="n">
+        <v>0.01060959640031973</v>
+      </c>
+      <c r="CI10" t="n">
+        <v>1.146456054960313</v>
+      </c>
+      <c r="CJ10" t="n">
+        <v>10.29291210992063</v>
+      </c>
+      <c r="CK10" t="n">
+        <v>8.730663759657029</v>
+      </c>
+      <c r="CL10" t="n">
+        <v>0.7515869735629384</v>
+      </c>
+      <c r="CM10" t="n">
+        <v>1</v>
+      </c>
+      <c r="CN10" t="n">
+        <v>44.06967878817415</v>
+      </c>
+      <c r="CO10" t="n">
+        <v>20.31071770134995</v>
+      </c>
+      <c r="CP10" t="n">
+        <v>0.01617613174917083</v>
+      </c>
+      <c r="CQ10" t="n">
+        <v>0.05982297849358999</v>
+      </c>
+      <c r="CR10" t="n">
+        <v>1.438688078856635</v>
+      </c>
+      <c r="CS10" t="n">
+        <v>12.87737615771327</v>
+      </c>
+      <c r="CT10" t="n">
+        <v>10.92456571988377</v>
+      </c>
+      <c r="CU10" t="n">
+        <v>0.6882664117639727</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>5c884b29c2ceec001719b1e4</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>lmp</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>neut</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G11" t="n">
+        <v>4.61512051684126</v>
+      </c>
+      <c r="H11" t="n">
+        <v>11.23024103368252</v>
+      </c>
+      <c r="I11" t="n">
+        <v>10.83967894611662</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>64.30460936535296</v>
+      </c>
+      <c r="L11" t="n">
+        <v>7.922875621513903</v>
+      </c>
+      <c r="M11" t="n">
+        <v>5.239178251437598</v>
+      </c>
+      <c r="N11" t="n">
+        <v>14.4783565028752</v>
+      </c>
+      <c r="O11" t="n">
+        <v>13.6972323277434</v>
+      </c>
+      <c r="P11" t="n">
+        <v>-0.1352202466477439</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>7.588500647080338</v>
+      </c>
+      <c r="R11" t="n">
+        <v>64.4005151841327</v>
+      </c>
+      <c r="S11" t="n">
+        <v>5.817382650810729</v>
+      </c>
+      <c r="T11" t="n">
+        <v>15.63476530162146</v>
+      </c>
+      <c r="U11" t="n">
+        <v>14.85364112648966</v>
+      </c>
+      <c r="V11" t="n">
+        <v>-0.2605050354768065</v>
+      </c>
+      <c r="W11" t="n">
+        <v>0.53827081967794</v>
+      </c>
+      <c r="X11" t="n">
+        <v>5.94939402768764</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>11.62289144971141</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>3.381575507031641</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>12.76315101406328</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>11.59146475136558</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>0.2672833797748572</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>0.2720200382626984</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>0.09933464214792176</v>
+      </c>
+      <c r="AF11" t="n">
+        <v>0.7707725537495197</v>
+      </c>
+      <c r="AG11" t="n">
+        <v>8.135212285510454</v>
+      </c>
+      <c r="AH11" t="n">
+        <v>58.22104294291046</v>
+      </c>
+      <c r="AI11" t="n">
+        <v>3.537523009682273</v>
+      </c>
+      <c r="AJ11" t="n">
+        <v>17.07504601936455</v>
+      </c>
+      <c r="AK11" t="n">
+        <v>15.12223558153505</v>
+      </c>
+      <c r="AL11" t="n">
+        <v>0.233492820659108</v>
+      </c>
+      <c r="AM11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN11" t="n">
+        <v>10</v>
+      </c>
+      <c r="AO11" t="n">
+        <v>44.51054459537107</v>
+      </c>
+      <c r="AP11" t="n">
+        <v>40</v>
+      </c>
+      <c r="AQ11" t="n">
+        <v>4.615120506741259</v>
+      </c>
+      <c r="AR11" t="n">
+        <v>17.23024101348252</v>
+      </c>
+      <c r="AS11" t="n">
+        <v>15.66799266321892</v>
+      </c>
+      <c r="AT11" t="n">
+        <v>2.188458747554023e-09</v>
+      </c>
+      <c r="AU11" t="n">
+        <v>0.8066301965101784</v>
+      </c>
+      <c r="AV11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW11" t="n">
+        <v>8.118641700412406</v>
+      </c>
+      <c r="AX11" t="n">
+        <v>8.116492183424429</v>
+      </c>
+      <c r="AY11" t="n">
+        <v>45.01503890118956</v>
+      </c>
+      <c r="AZ11" t="n">
+        <v>43.11893224374796</v>
+      </c>
+      <c r="BA11" t="n">
+        <v>54.63425596757398</v>
+      </c>
+      <c r="BB11" t="n">
+        <v>4.731056683856171</v>
+      </c>
+      <c r="BC11" t="n">
+        <v>23.46211336771234</v>
+      </c>
+      <c r="BD11" t="n">
+        <v>20.72817875475105</v>
+      </c>
+      <c r="BE11" t="n">
+        <v>-0.02512094030737511</v>
+      </c>
+      <c r="BF11" t="n">
+        <v>0.1187264212806394</v>
+      </c>
+      <c r="BG11" t="n">
+        <v>7.108703026009351</v>
+      </c>
+      <c r="BH11" t="n">
+        <v>85.62936666154985</v>
+      </c>
+      <c r="BI11" t="n">
+        <v>1.009709657822516</v>
+      </c>
+      <c r="BJ11" t="n">
+        <v>2.747861023974903</v>
+      </c>
+      <c r="BK11" t="n">
+        <v>13.49572204794981</v>
+      </c>
+      <c r="BL11" t="n">
+        <v>11.93347369768621</v>
+      </c>
+      <c r="BM11" t="n">
+        <v>0.404596041653181</v>
+      </c>
+      <c r="BN11" t="n">
+        <v>0.1051171373314944</v>
+      </c>
+      <c r="BO11" t="n">
+        <v>8.02415563362247</v>
+      </c>
+      <c r="BP11" t="n">
+        <v>77.27888898750246</v>
+      </c>
+      <c r="BQ11" t="n">
+        <v>1.471755593388159</v>
+      </c>
+      <c r="BR11" t="n">
+        <v>0.6637177301688514</v>
+      </c>
+      <c r="BS11" t="n">
+        <v>4.721890495656955</v>
+      </c>
+      <c r="BT11" t="n">
+        <v>19.44378099131391</v>
+      </c>
+      <c r="BU11" t="n">
+        <v>17.49097055348441</v>
+      </c>
+      <c r="BV11" t="n">
+        <v>-0.02313481921567932</v>
+      </c>
+      <c r="BW11" t="n">
+        <v>5.873904867626222</v>
+      </c>
+      <c r="BX11" t="n">
+        <v>35.80566559389575</v>
+      </c>
+      <c r="BY11" t="n">
+        <v>39.30849904554444</v>
+      </c>
+      <c r="BZ11" t="n">
+        <v>0.2540266495878884</v>
+      </c>
+      <c r="CA11" t="n">
+        <v>5.419823801449112</v>
+      </c>
+      <c r="CB11" t="n">
+        <v>18.83964760289822</v>
+      </c>
+      <c r="CC11" t="n">
+        <v>17.27739925263463</v>
+      </c>
+      <c r="CD11" t="n">
+        <v>-0.1743623555812618</v>
+      </c>
+      <c r="CE11" t="n">
+        <v>6.371798107810487</v>
+      </c>
+      <c r="CF11" t="n">
+        <v>56.27335564428358</v>
+      </c>
+      <c r="CG11" t="n">
+        <v>74.7828618918888</v>
+      </c>
+      <c r="CH11" t="n">
+        <v>0.6810622783526229</v>
+      </c>
+      <c r="CI11" t="n">
+        <v>7.126269569950428</v>
+      </c>
+      <c r="CJ11" t="n">
+        <v>22.25253913990086</v>
+      </c>
+      <c r="CK11" t="n">
+        <v>20.69029078963726</v>
+      </c>
+      <c r="CL11" t="n">
+        <v>-0.5441134297459</v>
+      </c>
+      <c r="CM11" t="n">
+        <v>5.958498293142919</v>
+      </c>
+      <c r="CN11" t="n">
+        <v>18.60143859158635</v>
+      </c>
+      <c r="CO11" t="n">
+        <v>70.90753548994807</v>
+      </c>
+      <c r="CP11" t="n">
+        <v>0.7075792085622322</v>
+      </c>
+      <c r="CQ11" t="n">
+        <v>0.2142209352050651</v>
+      </c>
+      <c r="CR11" t="n">
+        <v>2.806344646562009</v>
+      </c>
+      <c r="CS11" t="n">
+        <v>15.61268929312402</v>
+      </c>
+      <c r="CT11" t="n">
+        <v>13.65987885529452</v>
+      </c>
+      <c r="CU11" t="n">
+        <v>0.391923864973571</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>5c884b29c2ceec001719b1e4</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>lmfp</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>neut</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>5</v>
+      </c>
+      <c r="G12" t="n">
+        <v>4.61512051684126</v>
+      </c>
+      <c r="H12" t="n">
+        <v>11.23024103368252</v>
+      </c>
+      <c r="I12" t="n">
+        <v>10.83967894611662</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>53.08213395797932</v>
+      </c>
+      <c r="L12" t="n">
+        <v>3.655722393434712</v>
+      </c>
+      <c r="M12" t="n">
+        <v>7.118635246182857</v>
+      </c>
+      <c r="N12" t="n">
+        <v>18.23727049236571</v>
+      </c>
+      <c r="O12" t="n">
+        <v>17.45614631723392</v>
+      </c>
+      <c r="P12" t="n">
+        <v>-0.5424592316074742</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>6.408453094804099</v>
+      </c>
+      <c r="R12" t="n">
+        <v>39.82994673769347</v>
+      </c>
+      <c r="S12" t="n">
+        <v>3.194446904430232</v>
+      </c>
+      <c r="T12" t="n">
+        <v>10.38889380886046</v>
+      </c>
+      <c r="U12" t="n">
+        <v>9.607769633728665</v>
+      </c>
+      <c r="V12" t="n">
+        <v>0.3078302304840748</v>
+      </c>
+      <c r="W12" t="n">
+        <v>0.3641952991179447</v>
+      </c>
+      <c r="X12" t="n">
+        <v>1.992573318777873</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>38.88145923567979</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>2.237038952150364</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>10.47407790430073</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>9.302391641603029</v>
+      </c>
+      <c r="AC12" t="n">
+        <v>0.515280490728882</v>
+      </c>
+      <c r="AD12" t="n">
+        <v>0.781831390898076</v>
+      </c>
+      <c r="AE12" t="n">
+        <v>0.01828725497285799</v>
+      </c>
+      <c r="AF12" t="n">
+        <v>0.3913622164669825</v>
+      </c>
+      <c r="AG12" t="n">
+        <v>4.391402881044179</v>
+      </c>
+      <c r="AH12" t="n">
+        <v>55.75083022918069</v>
+      </c>
+      <c r="AI12" t="n">
+        <v>4.240519504179193</v>
+      </c>
+      <c r="AJ12" t="n">
+        <v>18.48103900835839</v>
+      </c>
+      <c r="AK12" t="n">
+        <v>16.52822857052889</v>
+      </c>
+      <c r="AL12" t="n">
+        <v>0.08116819729736018</v>
+      </c>
+      <c r="AM12" t="n">
+        <v>0.4020471949437128</v>
+      </c>
+      <c r="AN12" t="n">
+        <v>9.901873408242693</v>
+      </c>
+      <c r="AO12" t="n">
+        <v>51.11836213279485</v>
+      </c>
+      <c r="AP12" t="n">
+        <v>198.3157399039247</v>
+      </c>
+      <c r="AQ12" t="n">
+        <v>2.98202153260201</v>
+      </c>
+      <c r="AR12" t="n">
+        <v>13.96404306520402</v>
+      </c>
+      <c r="AS12" t="n">
+        <v>12.40179471494042</v>
+      </c>
+      <c r="AT12" t="n">
+        <v>0.3538583615053668</v>
+      </c>
+      <c r="AU12" t="n">
+        <v>0.7312471994244344</v>
+      </c>
+      <c r="AV12" t="n">
+        <v>0.2927906215436712</v>
+      </c>
+      <c r="AW12" t="n">
+        <v>4.992438560628749</v>
+      </c>
+      <c r="AX12" t="n">
+        <v>7.441684326856489</v>
+      </c>
+      <c r="AY12" t="n">
+        <v>11.11747535197416</v>
+      </c>
+      <c r="AZ12" t="n">
+        <v>45.76732886508131</v>
+      </c>
+      <c r="BA12" t="n">
+        <v>108.7864849079153</v>
+      </c>
+      <c r="BB12" t="n">
+        <v>5.697211347626692</v>
+      </c>
+      <c r="BC12" t="n">
+        <v>25.39442269525338</v>
+      </c>
+      <c r="BD12" t="n">
+        <v>22.66048808229209</v>
+      </c>
+      <c r="BE12" t="n">
+        <v>-0.2344664298227365</v>
+      </c>
+      <c r="BF12" t="n">
+        <v>0.08489128000775104</v>
+      </c>
+      <c r="BG12" t="n">
+        <v>1.948640513859567</v>
+      </c>
+      <c r="BH12" t="n">
+        <v>68.94145381036242</v>
+      </c>
+      <c r="BI12" t="n">
+        <v>0.54743349592718</v>
+      </c>
+      <c r="BJ12" t="n">
+        <v>5.513746309384785</v>
+      </c>
+      <c r="BK12" t="n">
+        <v>19.02749261876957</v>
+      </c>
+      <c r="BL12" t="n">
+        <v>17.46524426850597</v>
+      </c>
+      <c r="BM12" t="n">
+        <v>-0.1947133968147321</v>
+      </c>
+      <c r="BN12" t="n">
+        <v>0.09749276571256067</v>
+      </c>
+      <c r="BO12" t="n">
+        <v>2.834210906619603</v>
+      </c>
+      <c r="BP12" t="n">
+        <v>64.43964168797612</v>
+      </c>
+      <c r="BQ12" t="n">
+        <v>1.422219629224776</v>
+      </c>
+      <c r="BR12" t="n">
+        <v>0.8211677159673587</v>
+      </c>
+      <c r="BS12" t="n">
+        <v>1.844886957936044</v>
+      </c>
+      <c r="BT12" t="n">
+        <v>13.68977391587209</v>
+      </c>
+      <c r="BU12" t="n">
+        <v>11.73696347804259</v>
+      </c>
+      <c r="BV12" t="n">
+        <v>0.6002516183047056</v>
+      </c>
+      <c r="BW12" t="n">
+        <v>6.060597839623678</v>
+      </c>
+      <c r="BX12" t="n">
+        <v>46.20352395612262</v>
+      </c>
+      <c r="BY12" t="n">
+        <v>71.84841522569525</v>
+      </c>
+      <c r="BZ12" t="n">
+        <v>0.2360776681586751</v>
+      </c>
+      <c r="CA12" t="n">
+        <v>6.131053446045616</v>
+      </c>
+      <c r="CB12" t="n">
+        <v>20.26210689209124</v>
+      </c>
+      <c r="CC12" t="n">
+        <v>18.69985854182763</v>
+      </c>
+      <c r="CD12" t="n">
+        <v>-0.3284709302113546</v>
+      </c>
+      <c r="CE12" t="n">
+        <v>1.40464160319237</v>
+      </c>
+      <c r="CF12" t="n">
+        <v>37.72555214357309</v>
+      </c>
+      <c r="CG12" t="n">
+        <v>67.99515792041815</v>
+      </c>
+      <c r="CH12" t="n">
+        <v>0.2781978005368349</v>
+      </c>
+      <c r="CI12" t="n">
+        <v>1.902068015175674</v>
+      </c>
+      <c r="CJ12" t="n">
+        <v>11.80413603035135</v>
+      </c>
+      <c r="CK12" t="n">
+        <v>10.24188768008775</v>
+      </c>
+      <c r="CL12" t="n">
+        <v>0.5878616802671252</v>
+      </c>
+      <c r="CM12" t="n">
+        <v>1.328140448192499</v>
+      </c>
+      <c r="CN12" t="n">
+        <v>43.00154687114585</v>
+      </c>
+      <c r="CO12" t="n">
+        <v>67.33107536557024</v>
+      </c>
+      <c r="CP12" t="n">
+        <v>0.2693706180774156</v>
+      </c>
+      <c r="CQ12" t="n">
+        <v>0</v>
+      </c>
+      <c r="CR12" t="n">
+        <v>2.231659565946996</v>
+      </c>
+      <c r="CS12" t="n">
+        <v>14.46331913189399</v>
+      </c>
+      <c r="CT12" t="n">
+        <v>12.51050869406449</v>
+      </c>
+      <c r="CU12" t="n">
+        <v>0.5164460911035066</v>
       </c>
     </row>
   </sheetData>

</xml_diff>